<commit_message>
Updated with one possible future...
</commit_message>
<xml_diff>
--- a/misc/klask-burn-up.xlsx
+++ b/misc/klask-burn-up.xlsx
@@ -1,35 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\student\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsteele/Documents/2020-spring-jsf-m/klask/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E579DD-555B-A041-BD92-E3AF99AF3782}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="12300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data-entry" sheetId="1" r:id="rId1"/>
     <sheet name="backlog-breakdown" sheetId="2" r:id="rId2"/>
     <sheet name="burn-up" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="57" r:id="rId4"/>
+    <pivotCache cacheId="15" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="45">
   <si>
     <t>Date</t>
   </si>
@@ -161,12 +170,18 @@
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>web-api</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -196,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -210,6 +225,8 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -222,7 +239,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -277,7 +294,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -339,27 +355,12 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:forward val="100"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>'burn-up'!$F$4:$F$6</c:f>
+              <c:f>'burn-up'!$F$4:$F$8</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>43892</c:v>
                 </c:pt>
@@ -369,15 +370,21 @@
                 <c:pt idx="2">
                   <c:v>43902</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>43920</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="d\-mmm">
+                  <c:v>43997</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'burn-up'!$G$4:$G$6</c:f>
+              <c:f>'burn-up'!$G$4:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>39.5</c:v>
                 </c:pt>
@@ -386,6 +393,12 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>39.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -440,10 +453,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>'burn-up'!$F$4:$F$6</c:f>
+              <c:f>'burn-up'!$F$4:$F$8</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>43892</c:v>
                 </c:pt>
@@ -453,15 +466,21 @@
                 <c:pt idx="2">
                   <c:v>43902</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>43920</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="d\-mmm">
+                  <c:v>43997</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'burn-up'!$H$4:$H$6</c:f>
+              <c:f>'burn-up'!$H$4:$H$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -470,6 +489,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -497,7 +519,7 @@
         <c:axId val="472557808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="43966"/>
+          <c:max val="43997"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -515,7 +537,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1234,7 +1256,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1253,16 +1281,18 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="student" refreshedDate="43902.684811226849" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="30">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="43920.562164930554" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="36" xr:uid="{00000000-000A-0000-FFFF-FFFF39000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
   <cacheFields count="6">
-    <cacheField name="Date" numFmtId="14">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2020-03-02T00:00:00" maxDate="2020-03-13T00:00:00" count="3">
+    <cacheField name="Date" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2020-03-02T00:00:00" maxDate="2020-03-31T00:00:00" count="5">
         <d v="2020-03-02T00:00:00"/>
         <d v="2020-03-11T00:00:00"/>
         <d v="2020-03-12T00:00:00"/>
+        <d v="2020-03-30T00:00:00"/>
+        <d v="2020-03-26T00:00:00" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="level-1" numFmtId="0">
@@ -1276,7 +1306,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="level-2" numFmtId="0">
-      <sharedItems count="25">
+      <sharedItems count="26">
         <s v="ionic-info"/>
         <s v="mob-programming"/>
         <s v="research-bracket"/>
@@ -1302,13 +1332,14 @@
         <s v="choose-db"/>
         <s v="css-aesthetics"/>
         <s v="tourney-recruiting"/>
+        <s v="web-api"/>
       </sharedItems>
     </cacheField>
     <cacheField name="size-delta" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-3" maxValue="4"/>
     </cacheField>
     <cacheField name="release-target" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="4"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-3" maxValue="4"/>
     </cacheField>
     <cacheField name="work-completed" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="3"/>
@@ -1323,7 +1354,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="30">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="36">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -1564,18 +1595,68 @@
     <n v="0"/>
     <n v="1"/>
   </r>
+  <r>
+    <x v="3"/>
+    <x v="5"/>
+    <x v="22"/>
+    <n v="-3"/>
+    <n v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="5"/>
+    <x v="25"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="4"/>
+    <x v="20"/>
+    <n v="-3"/>
+    <n v="-3"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="4"/>
+    <x v="21"/>
+    <n v="-1.5"/>
+    <n v="0"/>
+    <n v="1.5"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="5"/>
+    <x v="24"/>
+    <n v="-0.5"/>
+    <n v="-0.5"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="18"/>
+    <n v="-1"/>
+    <n v="-1"/>
+    <n v="0"/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="57" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:E36" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:F37" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisCol" numFmtId="14" showAll="0">
-      <items count="4">
+      <items count="6">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
+        <item m="1" x="4"/>
+        <item x="3"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1591,7 +1672,7 @@
       </items>
     </pivotField>
     <pivotField axis="axisRow" showAll="0">
-      <items count="26">
+      <items count="27">
         <item x="6"/>
         <item x="3"/>
         <item x="8"/>
@@ -1617,6 +1698,7 @@
         <item x="22"/>
         <item x="23"/>
         <item x="24"/>
+        <item x="25"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1628,7 +1710,7 @@
     <field x="1"/>
     <field x="2"/>
   </rowFields>
-  <rowItems count="32">
+  <rowItems count="33">
     <i>
       <x/>
     </i>
@@ -1721,6 +1803,9 @@
     </i>
     <i r="1">
       <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="25"/>
     </i>
     <i t="grand">
       <x/>
@@ -1729,7 +1814,7 @@
   <colFields count="1">
     <field x="0"/>
   </colFields>
-  <colItems count="4">
+  <colItems count="5">
     <i>
       <x/>
     </i>
@@ -1738,6 +1823,9 @@
     </i>
     <i>
       <x v="2"/>
+    </i>
+    <i>
+      <x v="4"/>
     </i>
     <i t="grand">
       <x/>
@@ -1751,19 +1839,24 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="57" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:C6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable3" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" numFmtId="14" showAll="0">
-      <items count="4">
+      <items count="6">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
+        <item m="1" x="4"/>
+        <item x="3"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1776,7 +1869,7 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="3">
+  <rowItems count="4">
     <i>
       <x/>
     </i>
@@ -1785,6 +1878,9 @@
     </i>
     <i>
       <x v="2"/>
+    </i>
+    <i>
+      <x v="4"/>
     </i>
   </rowItems>
   <colFields count="1">
@@ -1807,22 +1903,25 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F31" totalsRowShown="0">
-  <autoFilter ref="A1:F31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F37" totalsRowShown="0">
+  <autoFilter ref="A1:F37" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Date" dataDxfId="2"/>
-    <tableColumn id="2" name="level-1"/>
-    <tableColumn id="3" name="level-2"/>
-    <tableColumn id="4" name="size-delta"/>
-    <tableColumn id="5" name="release-target" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="level-1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="level-2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="size-delta"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="release-target" dataDxfId="1">
       <calculatedColumnFormula>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="work-completed" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="work-completed" dataDxfId="0">
       <calculatedColumnFormula>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2092,24 +2191,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2129,7 +2228,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43892</v>
       </c>
@@ -2151,7 +2250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43892</v>
       </c>
@@ -2173,7 +2272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43892</v>
       </c>
@@ -2195,7 +2294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43892</v>
       </c>
@@ -2217,7 +2316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43892</v>
       </c>
@@ -2239,7 +2338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43892</v>
       </c>
@@ -2261,7 +2360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43892</v>
       </c>
@@ -2283,7 +2382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43892</v>
       </c>
@@ -2305,7 +2404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43892</v>
       </c>
@@ -2327,7 +2426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43892</v>
       </c>
@@ -2349,7 +2448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43892</v>
       </c>
@@ -2371,7 +2470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>43892</v>
       </c>
@@ -2393,7 +2492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43892</v>
       </c>
@@ -2415,7 +2514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43892</v>
       </c>
@@ -2437,7 +2536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43892</v>
       </c>
@@ -2459,7 +2558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43892</v>
       </c>
@@ -2481,7 +2580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43892</v>
       </c>
@@ -2503,7 +2602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43892</v>
       </c>
@@ -2525,7 +2624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43892</v>
       </c>
@@ -2547,7 +2646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43892</v>
       </c>
@@ -2569,7 +2668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43892</v>
       </c>
@@ -2591,7 +2690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43892</v>
       </c>
@@ -2613,7 +2712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>43892</v>
       </c>
@@ -2635,7 +2734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>43892</v>
       </c>
@@ -2657,7 +2756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>43892</v>
       </c>
@@ -2679,7 +2778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>43901</v>
       </c>
@@ -2701,7 +2800,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>43901</v>
       </c>
@@ -2723,7 +2822,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>43902</v>
       </c>
@@ -2745,7 +2844,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>43902</v>
       </c>
@@ -2767,7 +2866,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>43902</v>
       </c>
@@ -2787,6 +2886,135 @@
       <c r="F31" s="6">
         <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
         <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="7">
+        <v>43920</v>
+      </c>
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32">
+        <v>-3</v>
+      </c>
+      <c r="E32" s="6">
+        <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="F32" s="6">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="7">
+        <v>43920</v>
+      </c>
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33" s="6">
+        <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
+        <v>2</v>
+      </c>
+      <c r="F33" s="6">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="7">
+        <v>43920</v>
+      </c>
+      <c r="B34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34">
+        <v>-3</v>
+      </c>
+      <c r="E34" s="6">
+        <v>-3</v>
+      </c>
+      <c r="F34" s="6">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="7">
+        <v>43920</v>
+      </c>
+      <c r="B35" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35">
+        <v>-1.5</v>
+      </c>
+      <c r="E35" s="6">
+        <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="6">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="7">
+        <v>43920</v>
+      </c>
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36">
+        <v>-0.5</v>
+      </c>
+      <c r="E36" s="6">
+        <v>-0.5</v>
+      </c>
+      <c r="F36" s="6">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="7">
+        <v>43920</v>
+      </c>
+      <c r="B37" t="s">
+        <v>27</v>
+      </c>
+      <c r="C37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37">
+        <v>-1</v>
+      </c>
+      <c r="E37" s="6">
+        <v>-1</v>
+      </c>
+      <c r="F37" s="6">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2798,22 +3026,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:E36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A3:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -2821,7 +3049,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -2834,11 +3062,14 @@
       <c r="D4" s="1">
         <v>43902</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="1">
+        <v>43920</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -2851,11 +3082,12 @@
       <c r="D5" s="6">
         <v>-2</v>
       </c>
-      <c r="E5" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="6"/>
+      <c r="F5" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -2868,11 +3100,12 @@
       <c r="D6" s="6">
         <v>-1</v>
       </c>
-      <c r="E6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="6"/>
+      <c r="F6" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -2883,11 +3116,12 @@
       <c r="D7" s="6">
         <v>-0.5</v>
       </c>
-      <c r="E7" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="6"/>
+      <c r="F7" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -2898,11 +3132,12 @@
       <c r="D8" s="6">
         <v>-0.5</v>
       </c>
-      <c r="E8" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="6"/>
+      <c r="F8" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
@@ -2913,11 +3148,12 @@
         <v>-0.5</v>
       </c>
       <c r="D9" s="6"/>
-      <c r="E9" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="6"/>
+      <c r="F9" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
@@ -2926,11 +3162,12 @@
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="6">
+      <c r="E10" s="6"/>
+      <c r="F10" s="6">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -2939,11 +3176,12 @@
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="6">
+      <c r="E11" s="6"/>
+      <c r="F11" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -2952,11 +3190,12 @@
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="6">
+      <c r="E12" s="6"/>
+      <c r="F12" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
@@ -2965,11 +3204,12 @@
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="6">
+      <c r="E13" s="6"/>
+      <c r="F13" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>11</v>
       </c>
@@ -2978,11 +3218,12 @@
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
-      <c r="E14" s="6">
+      <c r="E14" s="6"/>
+      <c r="F14" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
@@ -2991,11 +3232,12 @@
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="6">
+      <c r="E15" s="6"/>
+      <c r="F15" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>13</v>
       </c>
@@ -3004,11 +3246,12 @@
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="6">
+      <c r="E16" s="6"/>
+      <c r="F16" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>16</v>
       </c>
@@ -3017,11 +3260,12 @@
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
-      <c r="E17" s="6">
+      <c r="E17" s="6"/>
+      <c r="F17" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
@@ -3030,11 +3274,12 @@
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
-      <c r="E18" s="6">
+      <c r="E18" s="6"/>
+      <c r="F18" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>22</v>
       </c>
@@ -3043,11 +3288,12 @@
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
-      <c r="E19" s="6">
+      <c r="E19" s="6"/>
+      <c r="F19" s="6">
         <v>5.5</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>23</v>
       </c>
@@ -3056,11 +3302,12 @@
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="6">
+      <c r="E20" s="6"/>
+      <c r="F20" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>24</v>
       </c>
@@ -3069,11 +3316,12 @@
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
-      <c r="E21" s="6">
+      <c r="E21" s="6"/>
+      <c r="F21" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>25</v>
       </c>
@@ -3082,11 +3330,12 @@
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
-      <c r="E22" s="6">
+      <c r="E22" s="6"/>
+      <c r="F22" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>26</v>
       </c>
@@ -3095,11 +3344,12 @@
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
-      <c r="E23" s="6">
+      <c r="E23" s="6"/>
+      <c r="F23" s="6">
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>27</v>
       </c>
@@ -3109,10 +3359,13 @@
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1</v>
+      </c>
+      <c r="F24" s="6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>28</v>
       </c>
@@ -3121,11 +3374,12 @@
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
-      <c r="E25" s="6">
+      <c r="E25" s="6"/>
+      <c r="F25" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>29</v>
       </c>
@@ -3134,11 +3388,12 @@
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
-      <c r="E26" s="6">
+      <c r="E26" s="6"/>
+      <c r="F26" s="6">
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>30</v>
       </c>
@@ -3148,10 +3403,13 @@
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1</v>
+      </c>
+      <c r="F27" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>31</v>
       </c>
@@ -3161,10 +3419,13 @@
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-4.5</v>
+      </c>
+      <c r="F28" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>32</v>
       </c>
@@ -3173,11 +3434,12 @@
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
-      <c r="E29" s="6">
+      <c r="E29" s="6"/>
+      <c r="F29" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>33</v>
       </c>
@@ -3187,10 +3449,13 @@
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-3</v>
+      </c>
+      <c r="F30" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>34</v>
       </c>
@@ -3200,10 +3465,13 @@
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1.5</v>
+      </c>
+      <c r="F31" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>35</v>
       </c>
@@ -3213,10 +3481,13 @@
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1.5</v>
+      </c>
+      <c r="F32" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>36</v>
       </c>
@@ -3226,10 +3497,13 @@
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-3</v>
+      </c>
+      <c r="F33" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>37</v>
       </c>
@@ -3238,11 +3512,12 @@
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
-      <c r="E34" s="6">
+      <c r="E34" s="6"/>
+      <c r="F34" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>38</v>
       </c>
@@ -3252,24 +3527,44 @@
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+        <v>-0.5</v>
+      </c>
+      <c r="F35" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6">
+        <v>2</v>
+      </c>
+      <c r="F36" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B37" s="6">
         <v>39.5</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C37" s="6">
         <v>-3.5</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D37" s="6">
         <v>-2</v>
       </c>
-      <c r="E36" s="6">
-        <v>34</v>
+      <c r="E37" s="6">
+        <v>-7</v>
+      </c>
+      <c r="F37" s="6">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -3278,24 +3573,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A3:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:G6"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -3315,7 +3610,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>43892</v>
       </c>
@@ -3326,19 +3621,19 @@
         <v>0</v>
       </c>
       <c r="F4" s="1">
-        <f>A4</f>
+        <f t="shared" ref="F4:H6" si="0">A4</f>
         <v>43892</v>
       </c>
       <c r="G4">
-        <f>B4</f>
+        <f t="shared" si="0"/>
         <v>39.5</v>
       </c>
       <c r="H4">
-        <f>C4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>43901</v>
       </c>
@@ -3349,19 +3644,19 @@
         <v>3.5</v>
       </c>
       <c r="F5" s="1">
-        <f>A5</f>
+        <f t="shared" si="0"/>
         <v>43901</v>
       </c>
       <c r="G5">
-        <f>B5</f>
+        <f t="shared" si="0"/>
         <v>39.5</v>
       </c>
       <c r="H5">
-        <f>C5</f>
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>43902</v>
       </c>
@@ -3372,16 +3667,47 @@
         <v>5.5</v>
       </c>
       <c r="F6" s="1">
-        <f>A6</f>
+        <f t="shared" si="0"/>
         <v>43902</v>
       </c>
       <c r="G6">
-        <f>B6</f>
+        <f t="shared" si="0"/>
         <v>39.5</v>
       </c>
       <c r="H6">
-        <f>C6</f>
+        <f t="shared" si="0"/>
         <v>5.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>43920</v>
+      </c>
+      <c r="B7" s="6">
+        <v>37</v>
+      </c>
+      <c r="C7" s="6">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" ref="F7" si="1">A7</f>
+        <v>43920</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ref="G7" si="2">B7</f>
+        <v>37</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ref="H7" si="3">C7</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F8" s="8">
+        <v>43997</v>
+      </c>
+      <c r="G8">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prepping for today's restart meeting...
</commit_message>
<xml_diff>
--- a/misc/klask-burn-up.xlsx
+++ b/misc/klask-burn-up.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsteele/Documents/2020-spring-jsf-m/klask/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8962F83-0226-1A43-B6D3-3F8E0C8F6C62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB84E86D-439E-6345-9ABB-09E9458A1F23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="12300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="12300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data-entry" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="45">
   <si>
     <t>Date</t>
   </si>
@@ -192,12 +192,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -212,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -226,11 +232,38 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1647,8 +1680,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="total" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="work-buckets" colHeaderCaption="date">
-  <location ref="A3:F11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="total" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="work-buckets" colHeaderCaption="date">
+  <location ref="A3:F23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisCol" numFmtId="165" showAll="0">
       <items count="7">
@@ -1664,8 +1697,8 @@
     <pivotField axis="axisRow" showAll="0">
       <items count="7">
         <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
+        <item x="1"/>
+        <item x="2"/>
         <item sd="0" x="3"/>
         <item sd="0" x="4"/>
         <item sd="0" x="5"/>
@@ -1711,15 +1744,51 @@
     <field x="1"/>
     <field x="2"/>
   </rowFields>
-  <rowItems count="7">
+  <rowItems count="19">
     <i>
       <x/>
     </i>
     <i>
       <x v="1"/>
     </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+    </i>
     <i>
       <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x v="14"/>
+    </i>
+    <i r="1">
+      <x v="15"/>
     </i>
     <i>
       <x v="3"/>
@@ -1757,6 +1826,32 @@
   <dataFields count="1">
     <dataField name="backlog-breakdown" fld="3" baseField="0" baseItem="0"/>
   </dataFields>
+  <formats count="2">
+    <format dxfId="2">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="2" count="1">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="0">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="2" count="1">
+            <x v="12"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -1770,7 +1865,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" numFmtId="14" showAll="0">
@@ -1838,14 +1933,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F37" totalsRowShown="0">
   <autoFilter ref="A1:F37" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="level-1"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="level-2"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="size-delta"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="release-target" dataDxfId="1">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="release-target" dataDxfId="4">
       <calculatedColumnFormula>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="work-completed" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="work-completed" dataDxfId="3">
       <calculatedColumnFormula>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2950,15 +3045,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A3:F11"/>
+  <dimension ref="A3:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.5" bestFit="1" customWidth="1"/>
@@ -3026,84 +3121,252 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>19</v>
+      <c r="A7" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="B7" s="5">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5">
-        <v>5.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>24</v>
+      <c r="A8" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="B8" s="5">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="5">
-        <v>-1</v>
-      </c>
+      <c r="E8" s="5"/>
       <c r="F8" s="5">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>28</v>
+      <c r="A9" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="B9" s="5">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
-      <c r="E9" s="5">
-        <v>-4.5</v>
-      </c>
+      <c r="E9" s="5"/>
       <c r="F9" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="5">
         <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="5">
-        <v>6.5</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="5">
+      <c r="E10" s="5"/>
+      <c r="F10" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="5">
+        <v>2</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="5">
+        <v>1</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="5">
+        <v>5.5</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="5">
+        <v>1</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="5">
+        <v>3</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="5">
+        <v>1</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F20" s="5">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="5">
+        <v>5.5</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5">
+        <v>-4.5</v>
+      </c>
+      <c r="F21" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="5">
+        <v>6.5</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5">
         <v>-1.5</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F22" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B23" s="5">
         <v>39.5</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C23" s="5">
         <v>-3.5</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D23" s="5">
         <v>-2</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E23" s="5">
         <v>-7</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F23" s="5">
         <v>27</v>
       </c>
     </row>
@@ -3116,7 +3379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A3:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated with Trevor's work
</commit_message>
<xml_diff>
--- a/misc/klask-burn-up.xlsx
+++ b/misc/klask-burn-up.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valer\Documents\GitHub\klask\misc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\molde\Documents\GitHub\klask\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F0B990-C708-4A23-9F13-82B9FCB4BEF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E757926B-7618-4BD5-86D4-91F7249A0BFB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,9 +28,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="45">
   <si>
     <t>Date</t>
   </si>
@@ -451,7 +449,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -489,10 +487,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'burn-up'!$F$4:$F$9</c:f>
+              <c:f>'burn-up'!$F$4:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>43892</c:v>
                 </c:pt>
@@ -508,7 +506,10 @@
                 <c:pt idx="4">
                   <c:v>43936</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="d\-mmm">
+                <c:pt idx="5">
+                  <c:v>43938</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="d\-mmm">
                   <c:v>44013</c:v>
                 </c:pt>
               </c:numCache>
@@ -516,10 +517,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'burn-up'!$G$4:$G$9</c:f>
+              <c:f>'burn-up'!$G$4:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>39.5</c:v>
                 </c:pt>
@@ -536,6 +537,9 @@
                   <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>36</c:v>
                 </c:pt>
               </c:numCache>
@@ -591,10 +595,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>'burn-up'!$F$4:$F$9</c:f>
+              <c:f>'burn-up'!$F$4:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>43892</c:v>
                 </c:pt>
@@ -610,7 +614,10 @@
                 <c:pt idx="4">
                   <c:v>43936</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="d\-mmm">
+                <c:pt idx="5">
+                  <c:v>43938</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="d\-mmm">
                   <c:v>44013</c:v>
                 </c:pt>
               </c:numCache>
@@ -618,10 +625,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'burn-up'!$H$4:$H$8</c:f>
+              <c:f>'burn-up'!$H$4:$H$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -636,6 +643,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -715,7 +725,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="472556976"/>
@@ -775,7 +785,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="472557808"/>
@@ -816,7 +826,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1388,15 +1398,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:colOff>1021080</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>541020</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1425,18 +1435,19 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Valeria Welsh" refreshedDate="43936.676343171297" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="39" xr:uid="{00000000-000A-0000-FFFF-FFFF39000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Trevor Moldenhauer" refreshedDate="43938.606083449071" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="40" xr:uid="{00000000-000A-0000-FFFF-FFFF39000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
   <cacheFields count="6">
     <cacheField name="Date" numFmtId="14">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2020-03-02T00:00:00" maxDate="2020-04-16T00:00:00" count="7">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2020-03-02T00:00:00" maxDate="2020-04-18T00:00:00" count="8">
         <d v="2020-03-02T00:00:00"/>
         <d v="2020-03-11T00:00:00"/>
         <d v="2020-03-12T00:00:00"/>
         <d v="2020-04-13T00:00:00"/>
         <d v="2020-04-15T00:00:00"/>
+        <d v="2020-04-17T00:00:00"/>
         <d v="2020-03-30T00:00:00" u="1"/>
         <d v="2020-03-26T00:00:00" u="1"/>
       </sharedItems>
@@ -1501,7 +1512,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="39">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="40">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -1814,22 +1825,31 @@
     <n v="0"/>
     <n v="2"/>
   </r>
+  <r>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="15"/>
+    <n v="-1"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="total" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="work-buckets" colHeaderCaption="date">
-  <location ref="A3:G23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <location ref="A3:H23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisCol" numFmtId="164" showAll="0">
-      <items count="8">
+      <items count="9">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
+        <item m="1" x="7"/>
         <item m="1" x="6"/>
-        <item m="1" x="5"/>
         <item x="3"/>
         <item x="4"/>
+        <item x="5"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1946,7 +1966,7 @@
   <colFields count="1">
     <field x="0"/>
   </colFields>
-  <colItems count="6">
+  <colItems count="7">
     <i>
       <x/>
     </i>
@@ -1961,6 +1981,9 @@
     </i>
     <i>
       <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
     </i>
     <i t="grand">
       <x/>
@@ -2076,17 +2099,18 @@
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:C8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <location ref="A3:C9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" numFmtId="14" showAll="0">
-      <items count="8">
+      <items count="9">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
+        <item m="1" x="7"/>
         <item m="1" x="6"/>
-        <item m="1" x="5"/>
         <item x="3"/>
         <item x="4"/>
+        <item x="5"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2099,7 +2123,7 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="5">
+  <rowItems count="6">
     <i>
       <x/>
     </i>
@@ -2114,6 +2138,9 @@
     </i>
     <i>
       <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
     </i>
   </rowItems>
   <colFields count="1">
@@ -2144,8 +2171,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F40" totalsRowShown="0">
-  <autoFilter ref="A1:F40" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F41" totalsRowShown="0">
+  <autoFilter ref="A1:F41" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="18"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="level-1"/>
@@ -2425,10 +2452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3315,6 +3342,28 @@
         <v>2</v>
       </c>
     </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="6">
+        <v>43938</v>
+      </c>
+      <c r="B41" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" t="s">
+        <v>44</v>
+      </c>
+      <c r="D41">
+        <v>-1</v>
+      </c>
+      <c r="E41" s="5">
+        <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="F41" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3325,21 +3374,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A3:G23"/>
+  <dimension ref="A3:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>41</v>
       </c>
@@ -3347,7 +3396,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>42</v>
       </c>
@@ -3366,11 +3415,14 @@
       <c r="F4" s="10">
         <v>43936</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="10">
+        <v>43938</v>
+      </c>
+      <c r="H4" s="10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -3385,11 +3437,12 @@
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G5" s="5"/>
+      <c r="H5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -3402,11 +3455,12 @@
       <c r="F6" s="5">
         <v>-2</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="5"/>
+      <c r="H6" s="5">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>12</v>
       </c>
@@ -3417,11 +3471,12 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="5">
+      <c r="G7" s="5"/>
+      <c r="H7" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>14</v>
       </c>
@@ -3432,11 +3487,12 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="5">
+      <c r="G8" s="5"/>
+      <c r="H8" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>17</v>
       </c>
@@ -3447,11 +3503,12 @@
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="5">
+      <c r="G9" s="5"/>
+      <c r="H9" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>11</v>
       </c>
@@ -3462,11 +3519,12 @@
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="5">
+      <c r="G10" s="5"/>
+      <c r="H10" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>10</v>
       </c>
@@ -3477,11 +3535,12 @@
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="5">
+      <c r="G11" s="5"/>
+      <c r="H11" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>13</v>
       </c>
@@ -3494,11 +3553,12 @@
       <c r="F12" s="5">
         <v>-2</v>
       </c>
-      <c r="G12" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G12" s="5"/>
+      <c r="H12" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>16</v>
       </c>
@@ -3509,11 +3569,12 @@
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="5">
+      <c r="G13" s="5"/>
+      <c r="H13" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
@@ -3524,11 +3585,12 @@
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="5">
+      <c r="G14" s="5"/>
+      <c r="H14" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
@@ -3542,10 +3604,13 @@
         <v>-0.5</v>
       </c>
       <c r="G15" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>-1</v>
+      </c>
+      <c r="H15" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>20</v>
       </c>
@@ -3558,11 +3623,12 @@
       <c r="F16" s="5">
         <v>-1</v>
       </c>
-      <c r="G16" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G16" s="5"/>
+      <c r="H16" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>21</v>
       </c>
@@ -3573,11 +3639,12 @@
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
-      <c r="G17" s="5">
+      <c r="G17" s="5"/>
+      <c r="H17" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>22</v>
       </c>
@@ -3588,11 +3655,12 @@
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="5">
+      <c r="G18" s="5"/>
+      <c r="H18" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>44</v>
       </c>
@@ -3606,10 +3674,13 @@
         <v>0.5</v>
       </c>
       <c r="G19" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+        <v>-1</v>
+      </c>
+      <c r="H19" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>23</v>
       </c>
@@ -3622,11 +3693,12 @@
         <v>-1</v>
       </c>
       <c r="F20" s="5"/>
-      <c r="G20" s="5">
+      <c r="G20" s="5"/>
+      <c r="H20" s="5">
         <v>1.5</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>27</v>
       </c>
@@ -3639,11 +3711,12 @@
         <v>-4.5</v>
       </c>
       <c r="F21" s="5"/>
-      <c r="G21" s="5">
+      <c r="G21" s="5"/>
+      <c r="H21" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>31</v>
       </c>
@@ -3656,11 +3729,12 @@
         <v>-1.5</v>
       </c>
       <c r="F22" s="5"/>
-      <c r="G22" s="5">
+      <c r="G22" s="5"/>
+      <c r="H22" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>43</v>
       </c>
@@ -3680,7 +3754,10 @@
         <v>-2.5</v>
       </c>
       <c r="G23" s="5">
-        <v>24.5</v>
+        <v>-1</v>
+      </c>
+      <c r="H23" s="5">
+        <v>23.5</v>
       </c>
     </row>
   </sheetData>
@@ -3690,10 +3767,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A3:H9"/>
+  <dimension ref="A3:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3842,10 +3919,33 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F9" s="7">
+      <c r="A9" s="3">
+        <v>43938</v>
+      </c>
+      <c r="B9" s="5">
+        <v>36</v>
+      </c>
+      <c r="C9" s="5">
+        <v>12.5</v>
+      </c>
+      <c r="F9" s="6">
+        <f t="shared" ref="F9" si="7">A9</f>
+        <v>43938</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ref="G9" si="8">B9</f>
+        <v>36</v>
+      </c>
+      <c r="H9">
+        <f t="shared" ref="H9" si="9">C9</f>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F10" s="7">
         <v>44013</v>
       </c>
-      <c r="G9">
+      <c r="G10">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reorganizing HTML... Updated burnup as well
</commit_message>
<xml_diff>
--- a/misc/klask-burn-up.xlsx
+++ b/misc/klask-burn-up.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\molde\Documents\GitHub\klask\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E757926B-7618-4BD5-86D4-91F7249A0BFB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{657AA7AE-BF33-4609-A164-D80B4A5B8752}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data-entry" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId4"/>
+    <pivotCache cacheId="15" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="45">
   <si>
     <t>Date</t>
   </si>
@@ -189,18 +189,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -210,7 +204,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -227,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -243,21 +237,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="96">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -313,7 +332,486 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d;@"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d;@"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d;@"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d;@"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d;@"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d;@"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d;@"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d;@"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -537,10 +1035,10 @@
                   <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>36</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -645,7 +1143,7 @@
                   <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.5</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1435,7 +1933,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Trevor Moldenhauer" refreshedDate="43938.606083449071" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="40" xr:uid="{00000000-000A-0000-FFFF-FFFF39000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Trevor Moldenhauer" refreshedDate="43938.631962500003" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="43" xr:uid="{00000000-000A-0000-FFFF-FFFF39000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
@@ -1448,8 +1946,8 @@
         <d v="2020-04-13T00:00:00"/>
         <d v="2020-04-15T00:00:00"/>
         <d v="2020-04-17T00:00:00"/>
+        <d v="2020-03-26T00:00:00" u="1"/>
         <d v="2020-03-30T00:00:00" u="1"/>
-        <d v="2020-03-26T00:00:00" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="level-1" numFmtId="0">
@@ -1512,7 +2010,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="40">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="43">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -1833,20 +2331,44 @@
     <n v="0"/>
     <n v="1"/>
   </r>
+  <r>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="13"/>
+    <n v="-3"/>
+    <n v="-3"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="14"/>
+    <n v="-1"/>
+    <n v="-1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="5"/>
+    <n v="-1"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="total" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="work-buckets" colHeaderCaption="date">
-  <location ref="A3:H23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="total" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="work-buckets" colHeaderCaption="date">
+  <location ref="A3:H29" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisCol" numFmtId="164" showAll="0">
       <items count="9">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
+        <item m="1" x="6"/>
         <item m="1" x="7"/>
-        <item m="1" x="6"/>
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
@@ -1857,10 +2379,10 @@
       <items count="7">
         <item sd="0" x="0"/>
         <item x="1"/>
-        <item x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
+        <item sd="0" x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1904,7 +2426,7 @@
     <field x="1"/>
     <field x="2"/>
   </rowFields>
-  <rowItems count="19">
+  <rowItems count="25">
     <i>
       <x/>
     </i>
@@ -1938,26 +2460,44 @@
     <i>
       <x v="2"/>
     </i>
-    <i r="1">
-      <x v="12"/>
+    <i>
+      <x v="3"/>
     </i>
     <i r="1">
-      <x v="13"/>
+      <x v="16"/>
     </i>
     <i r="1">
-      <x v="14"/>
+      <x v="17"/>
     </i>
     <i r="1">
-      <x v="26"/>
-    </i>
-    <i>
-      <x v="3"/>
+      <x v="18"/>
     </i>
     <i>
       <x v="4"/>
     </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i r="1">
+      <x v="20"/>
+    </i>
+    <i r="1">
+      <x v="21"/>
+    </i>
     <i>
       <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="22"/>
+    </i>
+    <i r="1">
+      <x v="23"/>
+    </i>
+    <i r="1">
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="25"/>
     </i>
     <i t="grand">
       <x/>
@@ -1992,8 +2532,8 @@
   <dataFields count="1">
     <dataField name="backlog-breakdown" fld="3" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="8">
-    <format dxfId="15">
+  <formats count="11">
+    <format dxfId="92">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2005,7 +2545,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="14">
+    <format dxfId="91">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2017,14 +2557,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="90">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="12">
+    <format dxfId="89">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2036,7 +2576,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="11">
+    <format dxfId="88">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2048,7 +2588,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="10">
+    <format dxfId="87">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2060,7 +2600,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="86">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2072,7 +2612,19 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="8">
+    <format dxfId="85">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="2" count="1">
+            <x v="26"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="3">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2080,6 +2632,30 @@
           </reference>
           <reference field="2" count="1">
             <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="2" count="1">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="0">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="2" count="1">
+            <x v="3"/>
           </reference>
         </references>
       </pivotArea>
@@ -2098,7 +2674,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable3" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" numFmtId="14" showAll="0">
@@ -2106,8 +2682,8 @@
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
+        <item m="1" x="6"/>
         <item m="1" x="7"/>
-        <item m="1" x="6"/>
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
@@ -2171,17 +2747,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F41" totalsRowShown="0">
-  <autoFilter ref="A1:F41" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F44" totalsRowShown="0">
+  <autoFilter ref="A1:F44" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="95"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="level-1"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="level-2"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="size-delta"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="release-target" dataDxfId="17">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="release-target" dataDxfId="94">
       <calculatedColumnFormula>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="work-completed" dataDxfId="16">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="work-completed" dataDxfId="93">
       <calculatedColumnFormula>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2452,10 +3028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3364,6 +3940,70 @@
         <v>1</v>
       </c>
     </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="6">
+        <v>43938</v>
+      </c>
+      <c r="B42" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D42">
+        <v>-3</v>
+      </c>
+      <c r="E42" s="5">
+        <v>-3</v>
+      </c>
+      <c r="F42" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="6">
+        <v>43938</v>
+      </c>
+      <c r="B43" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43">
+        <v>-1</v>
+      </c>
+      <c r="E43" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F43" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="6">
+        <v>43938</v>
+      </c>
+      <c r="B44" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44">
+        <v>-1</v>
+      </c>
+      <c r="E44" s="5">
+        <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="F44" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3374,15 +4014,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A3:H23"/>
+  <dimension ref="A3:H29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="4.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
@@ -3400,25 +4040,25 @@
       <c r="A4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>43892</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <v>43901</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <v>43902</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="9">
         <v>43934</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="9">
         <v>43936</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="9">
         <v>43938</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="9" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3455,9 +4095,11 @@
       <c r="F6" s="5">
         <v>-2</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="G6" s="5">
+        <v>-1</v>
+      </c>
       <c r="H6" s="5">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -3493,7 +4135,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="5">
@@ -3509,7 +4151,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="5">
@@ -3519,9 +4161,11 @@
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+      <c r="G10" s="5">
+        <v>-1</v>
+      </c>
       <c r="H10" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -3541,7 +4185,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="5">
@@ -3559,7 +4203,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="5">
@@ -3604,36 +4248,36 @@
         <v>-0.5</v>
       </c>
       <c r="G15" s="5">
-        <v>-1</v>
+        <v>-5</v>
       </c>
       <c r="H15" s="5">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
-        <v>20</v>
+      <c r="A16" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="B16" s="5">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5">
+      <c r="E16" s="5">
         <v>-1</v>
       </c>
+      <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B17" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -3641,15 +4285,15 @@
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B18" s="5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -3657,59 +4301,55 @@
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="5">
         <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="5">
-        <v>0.5</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="G19" s="5">
+      <c r="E19" s="5">
         <v>-1</v>
       </c>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
       <c r="H19" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B20" s="5">
-        <v>2.5</v>
+        <v>5.5</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5">
-        <v>-1</v>
+        <v>-4.5</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>27</v>
+      <c r="A21" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="B21" s="5">
-        <v>5.5</v>
+        <v>1</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="5">
-        <v>-4.5</v>
-      </c>
+      <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5">
@@ -3717,47 +4357,151 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>31</v>
+      <c r="A22" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="B22" s="5">
-        <v>6.5</v>
+        <v>3</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5">
-        <v>-1.5</v>
+        <v>-3</v>
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5">
+        <v>-1.5</v>
+      </c>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="5">
+        <v>6.5</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5">
+        <v>-1.5</v>
+      </c>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="5">
+        <v>3</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5">
+        <v>-3</v>
+      </c>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="5">
+        <v>3</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5">
+        <v>-0.5</v>
+      </c>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5">
+        <v>2</v>
+      </c>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B29" s="5">
         <v>39.5</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C29" s="5">
         <v>-3.5</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D29" s="5">
         <v>-2</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E29" s="5">
         <v>-7</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F29" s="5">
         <v>-2.5</v>
       </c>
-      <c r="G23" s="5">
-        <v>-1</v>
-      </c>
-      <c r="H23" s="5">
-        <v>23.5</v>
+      <c r="G29" s="5">
+        <v>-6</v>
+      </c>
+      <c r="H29" s="5">
+        <v>18.5</v>
       </c>
     </row>
   </sheetData>
@@ -3769,8 +4513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A3:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3923,10 +4667,10 @@
         <v>43938</v>
       </c>
       <c r="B9" s="5">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C9" s="5">
-        <v>12.5</v>
+        <v>13.5</v>
       </c>
       <c r="F9" s="6">
         <f t="shared" ref="F9" si="7">A9</f>
@@ -3934,11 +4678,11 @@
       </c>
       <c r="G9">
         <f t="shared" ref="G9" si="8">B9</f>
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H9">
         <f t="shared" ref="H9" si="9">C9</f>
-        <v>12.5</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -3946,7 +4690,7 @@
         <v>44013</v>
       </c>
       <c r="G10">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the burn-up chart and the readme file
</commit_message>
<xml_diff>
--- a/misc/klask-burn-up.xlsx
+++ b/misc/klask-burn-up.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\molde\Documents\GitHub\klask\misc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valer\Documents\GitHub\klask\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{657AA7AE-BF33-4609-A164-D80B4A5B8752}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C03DAD7-01A2-41FA-9B09-0C33C24DA579}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data-entry" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="15" r:id="rId4"/>
+    <pivotCache cacheId="5" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +28,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="45">
   <si>
     <t>Date</t>
   </si>
@@ -248,35 +250,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="96">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="25">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -325,7 +299,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -339,465 +313,28 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor theme="7" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d;@"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
+          <bgColor theme="7" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
+          <bgColor theme="7" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d;@"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d;@"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d;@"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d;@"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d;@"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d;@"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d;@"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor theme="7" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
     </dxf>
@@ -947,7 +484,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -985,10 +522,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'burn-up'!$F$4:$F$10</c:f>
+              <c:f>'burn-up'!$F$4:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>43892</c:v>
                 </c:pt>
@@ -1007,7 +544,10 @@
                 <c:pt idx="5">
                   <c:v>43938</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="d\-mmm">
+                <c:pt idx="6">
+                  <c:v>43941</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="d\-mmm">
                   <c:v>44013</c:v>
                 </c:pt>
               </c:numCache>
@@ -1015,10 +555,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'burn-up'!$G$4:$G$10</c:f>
+              <c:f>'burn-up'!$G$4:$G$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>39.5</c:v>
                 </c:pt>
@@ -1038,6 +578,9 @@
                   <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
@@ -1093,10 +636,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>'burn-up'!$F$4:$F$10</c:f>
+              <c:f>'burn-up'!$F$4:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>43892</c:v>
                 </c:pt>
@@ -1115,7 +658,10 @@
                 <c:pt idx="5">
                   <c:v>43938</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="d\-mmm">
+                <c:pt idx="6">
+                  <c:v>43941</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="d\-mmm">
                   <c:v>44013</c:v>
                 </c:pt>
               </c:numCache>
@@ -1123,10 +669,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'burn-up'!$H$4:$H$9</c:f>
+              <c:f>'burn-up'!$H$4:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1143,6 +689,9 @@
                   <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>13.5</c:v>
                 </c:pt>
               </c:numCache>
@@ -1223,7 +772,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="472556976"/>
@@ -1283,7 +832,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="472557808"/>
@@ -1324,7 +873,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1896,15 +1445,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1021080</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1933,21 +1482,22 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Trevor Moldenhauer" refreshedDate="43938.631962500003" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="43" xr:uid="{00000000-000A-0000-FFFF-FFFF39000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Valeria Welsh" refreshedDate="43941.619089583335" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="45" xr:uid="{00000000-000A-0000-FFFF-FFFF39000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
   <cacheFields count="6">
     <cacheField name="Date" numFmtId="14">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2020-03-02T00:00:00" maxDate="2020-04-18T00:00:00" count="8">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2020-03-02T00:00:00" maxDate="2020-04-21T00:00:00" count="9">
         <d v="2020-03-02T00:00:00"/>
         <d v="2020-03-11T00:00:00"/>
         <d v="2020-03-12T00:00:00"/>
         <d v="2020-04-13T00:00:00"/>
         <d v="2020-04-15T00:00:00"/>
         <d v="2020-04-17T00:00:00"/>
+        <d v="2020-04-20T00:00:00"/>
+        <d v="2020-03-30T00:00:00" u="1"/>
         <d v="2020-03-26T00:00:00" u="1"/>
-        <d v="2020-03-30T00:00:00" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="level-1" numFmtId="0">
@@ -2010,7 +1560,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="43">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="45">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -2355,23 +1905,40 @@
     <n v="0"/>
     <n v="1"/>
   </r>
+  <r>
+    <x v="6"/>
+    <x v="1"/>
+    <x v="10"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="1"/>
+    <x v="11"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="total" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="work-buckets" colHeaderCaption="date">
-  <location ref="A3:H29" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="total" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="work-buckets" colHeaderCaption="date">
+  <location ref="A3:I29" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisCol" numFmtId="164" showAll="0">
-      <items count="9">
+      <items count="10">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
-        <item m="1" x="6"/>
+        <item m="1" x="8"/>
         <item m="1" x="7"/>
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
+        <item x="6"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2506,7 +2073,7 @@
   <colFields count="1">
     <field x="0"/>
   </colFields>
-  <colItems count="7">
+  <colItems count="8">
     <i>
       <x/>
     </i>
@@ -2525,6 +2092,9 @@
     <i>
       <x v="7"/>
     </i>
+    <i>
+      <x v="8"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
@@ -2533,7 +2103,7 @@
     <dataField name="backlog-breakdown" fld="3" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="11">
-    <format dxfId="92">
+    <format dxfId="21">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2545,7 +2115,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="91">
+    <format dxfId="20">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2557,14 +2127,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="90">
+    <format dxfId="19">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="89">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2576,7 +2146,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="88">
+    <format dxfId="17">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2588,7 +2158,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="87">
+    <format dxfId="16">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2600,7 +2170,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="86">
+    <format dxfId="15">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2612,7 +2182,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="85">
+    <format dxfId="14">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2624,7 +2194,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="13">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2636,7 +2206,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2648,7 +2218,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="11">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2674,19 +2244,20 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable3" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:C9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" numFmtId="14" showAll="0">
-      <items count="9">
+      <items count="10">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
-        <item m="1" x="6"/>
+        <item m="1" x="8"/>
         <item m="1" x="7"/>
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
+        <item x="6"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2699,7 +2270,7 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="6">
+  <rowItems count="7">
     <i>
       <x/>
     </i>
@@ -2717,6 +2288,9 @@
     </i>
     <i>
       <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
     </i>
   </rowItems>
   <colFields count="1">
@@ -2747,17 +2321,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F44" totalsRowShown="0">
-  <autoFilter ref="A1:F44" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F46" totalsRowShown="0">
+  <autoFilter ref="A1:F46" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="95"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="level-1"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="level-2"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="size-delta"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="release-target" dataDxfId="94">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="release-target" dataDxfId="23">
       <calculatedColumnFormula>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="work-completed" dataDxfId="93">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="work-completed" dataDxfId="22">
       <calculatedColumnFormula>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3028,10 +2602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4004,6 +3578,50 @@
         <v>1</v>
       </c>
     </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="6">
+        <v>43941</v>
+      </c>
+      <c r="B45" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45" s="5">
+        <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="F45" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="6">
+        <v>43941</v>
+      </c>
+      <c r="B46" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" t="s">
+        <v>17</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46" s="5">
+        <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="F46" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -4014,21 +3632,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A3:H29"/>
+  <dimension ref="A3:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="8" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>41</v>
       </c>
@@ -4036,7 +3654,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>42</v>
       </c>
@@ -4058,11 +3676,14 @@
       <c r="G4" s="9">
         <v>43938</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="9">
+        <v>43941</v>
+      </c>
+      <c r="I4" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -4078,11 +3699,12 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H5" s="5"/>
+      <c r="I5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -4099,10 +3721,13 @@
         <v>-1</v>
       </c>
       <c r="H6" s="5">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>12</v>
       </c>
@@ -4114,11 +3739,12 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="5">
+      <c r="H7" s="5"/>
+      <c r="I7" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>14</v>
       </c>
@@ -4130,11 +3756,12 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="5">
+      <c r="H8" s="5"/>
+      <c r="I8" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>17</v>
       </c>
@@ -4147,10 +3774,13 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>11</v>
       </c>
@@ -4164,11 +3794,12 @@
       <c r="G10" s="5">
         <v>-1</v>
       </c>
-      <c r="H10" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H10" s="5"/>
+      <c r="I10" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>10</v>
       </c>
@@ -4180,11 +3811,12 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="5">
+      <c r="H11" s="5"/>
+      <c r="I11" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>13</v>
       </c>
@@ -4198,11 +3830,12 @@
         <v>-2</v>
       </c>
       <c r="G12" s="5"/>
-      <c r="H12" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H12" s="5"/>
+      <c r="I12" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>16</v>
       </c>
@@ -4215,10 +3848,13 @@
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5">
+        <v>0</v>
+      </c>
+      <c r="I13" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
@@ -4230,11 +3866,12 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="5">
+      <c r="H14" s="5"/>
+      <c r="I14" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
@@ -4250,11 +3887,12 @@
       <c r="G15" s="5">
         <v>-5</v>
       </c>
-      <c r="H15" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H15" s="5"/>
+      <c r="I15" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>23</v>
       </c>
@@ -4268,11 +3906,12 @@
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="5">
+      <c r="H16" s="5"/>
+      <c r="I16" s="5">
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>24</v>
       </c>
@@ -4284,11 +3923,12 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="5">
+      <c r="H17" s="5"/>
+      <c r="I17" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>25</v>
       </c>
@@ -4300,11 +3940,12 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
-      <c r="H18" s="5">
+      <c r="H18" s="5"/>
+      <c r="I18" s="5">
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>26</v>
       </c>
@@ -4318,11 +3959,12 @@
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H19" s="5"/>
+      <c r="I19" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>27</v>
       </c>
@@ -4336,11 +3978,12 @@
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="5">
+      <c r="H20" s="5"/>
+      <c r="I20" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>28</v>
       </c>
@@ -4352,11 +3995,12 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
-      <c r="H21" s="5">
+      <c r="H21" s="5"/>
+      <c r="I21" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>29</v>
       </c>
@@ -4370,11 +4014,12 @@
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
-      <c r="H22" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H22" s="5"/>
+      <c r="I22" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>30</v>
       </c>
@@ -4388,11 +4033,12 @@
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
-      <c r="H23" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H23" s="5"/>
+      <c r="I23" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>31</v>
       </c>
@@ -4406,11 +4052,12 @@
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
-      <c r="H24" s="5">
+      <c r="H24" s="5"/>
+      <c r="I24" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>32</v>
       </c>
@@ -4424,11 +4071,12 @@
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H25" s="5"/>
+      <c r="I25" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>33</v>
       </c>
@@ -4440,11 +4088,12 @@
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
-      <c r="H26" s="5">
+      <c r="H26" s="5"/>
+      <c r="I26" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>34</v>
       </c>
@@ -4458,11 +4107,12 @@
       </c>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
-      <c r="H27" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H27" s="5"/>
+      <c r="I27" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>40</v>
       </c>
@@ -4474,11 +4124,12 @@
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
-      <c r="H28" s="5">
+      <c r="H28" s="5"/>
+      <c r="I28" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>43</v>
       </c>
@@ -4501,6 +4152,9 @@
         <v>-6</v>
       </c>
       <c r="H29" s="5">
+        <v>0</v>
+      </c>
+      <c r="I29" s="5">
         <v>18.5</v>
       </c>
     </row>
@@ -4511,10 +4165,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A3:H10"/>
+  <dimension ref="A3:H11"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4686,10 +4340,33 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F10" s="7">
+      <c r="A10" s="3">
+        <v>43941</v>
+      </c>
+      <c r="B10" s="5">
+        <v>32</v>
+      </c>
+      <c r="C10" s="5">
+        <v>13.5</v>
+      </c>
+      <c r="F10" s="6">
+        <f t="shared" ref="F10" si="10">A10</f>
+        <v>43941</v>
+      </c>
+      <c r="G10">
+        <f t="shared" ref="G10" si="11">B10</f>
+        <v>32</v>
+      </c>
+      <c r="H10">
+        <f t="shared" ref="H10" si="12">C10</f>
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F11" s="7">
         <v>44013</v>
       </c>
-      <c r="G10">
+      <c r="G11">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating burnup for 4/24 meeting
</commit_message>
<xml_diff>
--- a/misc/klask-burn-up.xlsx
+++ b/misc/klask-burn-up.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trevo\OneDrive\Documents\GitHub\klask\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72164ECB-1CC9-43B4-A28F-5EE2CD0B02B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{678521D8-AB33-4E07-9513-5D23068D964F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2985" yWindow="2400" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data-entry" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="50" r:id="rId4"/>
+    <pivotCache cacheId="5" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="45">
   <si>
     <t>Date</t>
   </si>
@@ -250,883 +250,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="157">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d;@"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d;@"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d;@"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d;@"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d;@"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d;@"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d;@"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d;@"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d;@"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d;@"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d;@"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d;@"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="25">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1398,10 +522,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'burn-up'!$F$4:$F$12</c:f>
+              <c:f>'burn-up'!$F$4:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>43892</c:v>
                 </c:pt>
@@ -1426,7 +550,10 @@
                 <c:pt idx="7">
                   <c:v>43943</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="d\-mmm">
+                <c:pt idx="8">
+                  <c:v>43945</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="d\-mmm">
                   <c:v>44013</c:v>
                 </c:pt>
               </c:numCache>
@@ -1434,10 +561,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'burn-up'!$G$4:$G$12</c:f>
+              <c:f>'burn-up'!$G$4:$G$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>39.5</c:v>
                 </c:pt>
@@ -1463,6 +590,9 @@
                   <c:v>25.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>25.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>25.5</c:v>
                 </c:pt>
               </c:numCache>
@@ -1518,10 +648,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>'burn-up'!$F$4:$F$12</c:f>
+              <c:f>'burn-up'!$F$4:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>43892</c:v>
                 </c:pt>
@@ -1546,7 +676,10 @@
                 <c:pt idx="7">
                   <c:v>43943</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="d\-mmm">
+                <c:pt idx="8">
+                  <c:v>43945</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="d\-mmm">
                   <c:v>44013</c:v>
                 </c:pt>
               </c:numCache>
@@ -1554,10 +687,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'burn-up'!$H$4:$H$11</c:f>
+              <c:f>'burn-up'!$H$4:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1580,6 +713,9 @@
                   <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>15.5</c:v>
                 </c:pt>
               </c:numCache>
@@ -2370,13 +1506,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Trevor Moldenhauer" refreshedDate="43943.679817939817" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="52" xr:uid="{00000000-000A-0000-FFFF-FFFF39000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Trevor Moldenhauer" refreshedDate="43948.636545833331" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="53" xr:uid="{00000000-000A-0000-FFFF-FFFF39000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
   <cacheFields count="6">
     <cacheField name="Date" numFmtId="14">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2020-03-02T00:00:00" maxDate="2020-04-23T00:00:00" count="10">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2020-03-02T00:00:00" maxDate="2020-04-25T00:00:00" count="11">
         <d v="2020-03-02T00:00:00"/>
         <d v="2020-03-11T00:00:00"/>
         <d v="2020-03-12T00:00:00"/>
@@ -2385,8 +1521,9 @@
         <d v="2020-04-17T00:00:00"/>
         <d v="2020-04-20T00:00:00"/>
         <d v="2020-04-22T00:00:00"/>
+        <d v="2020-04-24T00:00:00"/>
+        <d v="2020-03-30T00:00:00" u="1"/>
         <d v="2020-03-26T00:00:00" u="1"/>
-        <d v="2020-03-30T00:00:00" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="level-1" numFmtId="0">
@@ -2449,7 +1586,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="52">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="53">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -2866,25 +2003,34 @@
     <n v="-2"/>
     <n v="0"/>
   </r>
+  <r>
+    <x v="8"/>
+    <x v="1"/>
+    <x v="11"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="50" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="total" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="work-buckets" colHeaderCaption="date">
-  <location ref="A3:J26" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="total" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="work-buckets" colHeaderCaption="date">
+  <location ref="A3:K26" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisCol" numFmtId="164" showAll="0">
-      <items count="11">
+      <items count="12">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
-        <item m="1" x="8"/>
+        <item m="1" x="10"/>
         <item m="1" x="9"/>
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
         <item x="6"/>
         <item x="7"/>
+        <item x="8"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -3010,7 +2156,7 @@
   <colFields count="1">
     <field x="0"/>
   </colFields>
-  <colItems count="9">
+  <colItems count="10">
     <i>
       <x/>
     </i>
@@ -3035,6 +2181,9 @@
     <i>
       <x v="9"/>
     </i>
+    <i>
+      <x v="10"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
@@ -3043,7 +2192,7 @@
     <dataField name="backlog-breakdown" fld="3" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="11">
-    <format dxfId="153">
+    <format dxfId="21">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3055,7 +2204,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="152">
+    <format dxfId="20">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3067,14 +2216,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="151">
+    <format dxfId="19">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="150">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3086,7 +2235,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="149">
+    <format dxfId="17">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3098,7 +2247,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="148">
+    <format dxfId="16">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3110,7 +2259,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="147">
+    <format dxfId="15">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3122,7 +2271,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="146">
+    <format dxfId="14">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3134,7 +2283,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="145">
+    <format dxfId="13">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3146,7 +2295,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="144">
+    <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3158,7 +2307,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="143">
+    <format dxfId="11">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -3184,21 +2333,22 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable3" cacheId="50" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" numFmtId="14" showAll="0">
-      <items count="11">
+      <items count="12">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
-        <item m="1" x="8"/>
+        <item m="1" x="10"/>
         <item m="1" x="9"/>
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
         <item x="6"/>
         <item x="7"/>
+        <item x="8"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -3211,7 +2361,7 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="8">
+  <rowItems count="9">
     <i>
       <x/>
     </i>
@@ -3235,6 +2385,9 @@
     </i>
     <i>
       <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
     </i>
   </rowItems>
   <colFields count="1">
@@ -3265,17 +2418,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F53" totalsRowShown="0">
-  <autoFilter ref="A1:F53" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F54" totalsRowShown="0">
+  <autoFilter ref="A1:F54" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="156"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="level-1"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="level-2"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="size-delta"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="release-target" dataDxfId="155">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="release-target" dataDxfId="23">
       <calculatedColumnFormula>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="work-completed" dataDxfId="154">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="work-completed" dataDxfId="22">
       <calculatedColumnFormula>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3546,10 +2699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E57" sqref="E56:E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4715,6 +3868,28 @@
         <v>0</v>
       </c>
     </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="6">
+        <v>43945</v>
+      </c>
+      <c r="B54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" t="s">
+        <v>17</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54" s="5">
+        <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="F54" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -4725,21 +3900,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A3:J26"/>
+  <dimension ref="A3:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>41</v>
       </c>
@@ -4747,7 +3922,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>42</v>
       </c>
@@ -4775,11 +3950,14 @@
       <c r="I4" s="9">
         <v>43943</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="9">
+        <v>43945</v>
+      </c>
+      <c r="K4" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -4797,11 +3975,12 @@
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J5" s="5"/>
+      <c r="K5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -4824,10 +4003,13 @@
         <v>-4</v>
       </c>
       <c r="J6" s="5">
+        <v>0</v>
+      </c>
+      <c r="K6" s="5">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>12</v>
       </c>
@@ -4841,11 +4023,12 @@
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
-      <c r="J7" s="5">
+      <c r="J7" s="5"/>
+      <c r="K7" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>14</v>
       </c>
@@ -4861,11 +4044,12 @@
       <c r="I8" s="5">
         <v>-2</v>
       </c>
-      <c r="J8" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J8" s="5"/>
+      <c r="K8" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>17</v>
       </c>
@@ -4884,10 +4068,13 @@
         <v>-1</v>
       </c>
       <c r="J9" s="5">
+        <v>0</v>
+      </c>
+      <c r="K9" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>11</v>
       </c>
@@ -4903,11 +4090,12 @@
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
-      <c r="J10" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J10" s="5"/>
+      <c r="K10" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>10</v>
       </c>
@@ -4923,11 +4111,12 @@
       <c r="I11" s="5">
         <v>-1</v>
       </c>
-      <c r="J11" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J11" s="5"/>
+      <c r="K11" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>13</v>
       </c>
@@ -4943,11 +4132,12 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
-      <c r="J12" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J12" s="5"/>
+      <c r="K12" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>16</v>
       </c>
@@ -4963,11 +4153,12 @@
         <v>0</v>
       </c>
       <c r="I13" s="5"/>
-      <c r="J13" s="5">
+      <c r="J13" s="5"/>
+      <c r="K13" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
@@ -4981,11 +4172,12 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
-      <c r="J14" s="5">
+      <c r="J14" s="5"/>
+      <c r="K14" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
@@ -5003,11 +4195,12 @@
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
-      <c r="J15" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J15" s="5"/>
+      <c r="K15" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>23</v>
       </c>
@@ -5025,11 +4218,12 @@
       <c r="I16" s="5">
         <v>-1.5</v>
       </c>
-      <c r="J16" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J16" s="5"/>
+      <c r="K16" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>27</v>
       </c>
@@ -5045,11 +4239,12 @@
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
-      <c r="J17" s="5">
+      <c r="J17" s="5"/>
+      <c r="K17" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>28</v>
       </c>
@@ -5063,11 +4258,12 @@
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
-      <c r="J18" s="5">
+      <c r="J18" s="5"/>
+      <c r="K18" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>29</v>
       </c>
@@ -5083,11 +4279,12 @@
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
-      <c r="J19" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J19" s="5"/>
+      <c r="K19" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>30</v>
       </c>
@@ -5103,11 +4300,12 @@
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
-      <c r="J20" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J20" s="5"/>
+      <c r="K20" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>31</v>
       </c>
@@ -5125,11 +4323,12 @@
       <c r="I21" s="5">
         <v>-3</v>
       </c>
-      <c r="J21" s="5">
+      <c r="J21" s="5"/>
+      <c r="K21" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>32</v>
       </c>
@@ -5145,11 +4344,12 @@
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
-      <c r="J22" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J22" s="5"/>
+      <c r="K22" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>33</v>
       </c>
@@ -5165,11 +4365,12 @@
       <c r="I23" s="5">
         <v>-1</v>
       </c>
-      <c r="J23" s="5">
+      <c r="J23" s="5"/>
+      <c r="K23" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>34</v>
       </c>
@@ -5185,11 +4386,12 @@
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
-      <c r="J24" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J24" s="5"/>
+      <c r="K24" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>40</v>
       </c>
@@ -5205,11 +4407,12 @@
       <c r="I25" s="5">
         <v>-2</v>
       </c>
-      <c r="J25" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J25" s="5"/>
+      <c r="K25" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>43</v>
       </c>
@@ -5238,6 +4441,9 @@
         <v>-8.5</v>
       </c>
       <c r="J26" s="5">
+        <v>0</v>
+      </c>
+      <c r="K26" s="5">
         <v>10</v>
       </c>
     </row>
@@ -5248,10 +4454,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A3:H12"/>
+  <dimension ref="A3:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5469,10 +4675,33 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F12" s="7">
+      <c r="A12" s="3">
+        <v>43945</v>
+      </c>
+      <c r="B12" s="5">
+        <v>25.5</v>
+      </c>
+      <c r="C12" s="5">
+        <v>15.5</v>
+      </c>
+      <c r="F12" s="6">
+        <f t="shared" ref="F12" si="16">A12</f>
+        <v>43945</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ref="G12" si="17">B12</f>
+        <v>25.5</v>
+      </c>
+      <c r="H12">
+        <f t="shared" ref="H12" si="18">C12</f>
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F13" s="7">
         <v>44013</v>
       </c>
-      <c r="G12">
+      <c r="G13">
         <v>25.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated burnup for 4/27 meeting
</commit_message>
<xml_diff>
--- a/misc/klask-burn-up.xlsx
+++ b/misc/klask-burn-up.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trevo\OneDrive\Documents\GitHub\klask\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{678521D8-AB33-4E07-9513-5D23068D964F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1643E8-4396-4069-93FD-B8366C26591A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="2400" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data-entry" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="45">
   <si>
     <t>Date</t>
   </si>
@@ -522,10 +522,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'burn-up'!$F$4:$F$13</c:f>
+              <c:f>'burn-up'!$F$4:$F$14</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>43892</c:v>
                 </c:pt>
@@ -553,7 +553,10 @@
                 <c:pt idx="8">
                   <c:v>43945</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="d\-mmm">
+                <c:pt idx="9">
+                  <c:v>43948</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="d\-mmm">
                   <c:v>44013</c:v>
                 </c:pt>
               </c:numCache>
@@ -561,10 +564,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'burn-up'!$G$4:$G$13</c:f>
+              <c:f>'burn-up'!$G$4:$G$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>39.5</c:v>
                 </c:pt>
@@ -593,6 +596,9 @@
                   <c:v>25.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>25.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>25.5</c:v>
                 </c:pt>
               </c:numCache>
@@ -648,10 +654,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>'burn-up'!$F$4:$F$13</c:f>
+              <c:f>'burn-up'!$F$4:$F$14</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>43892</c:v>
                 </c:pt>
@@ -679,7 +685,10 @@
                 <c:pt idx="8">
                   <c:v>43945</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="d\-mmm">
+                <c:pt idx="9">
+                  <c:v>43948</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="d\-mmm">
                   <c:v>44013</c:v>
                 </c:pt>
               </c:numCache>
@@ -687,10 +696,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'burn-up'!$H$4:$H$12</c:f>
+              <c:f>'burn-up'!$H$4:$H$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -717,6 +726,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1468,16 +1480,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1483995</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>182880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>558165</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1506,13 +1518,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Trevor Moldenhauer" refreshedDate="43948.636545833331" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="53" xr:uid="{00000000-000A-0000-FFFF-FFFF39000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Trevor Moldenhauer" refreshedDate="43948.638872337964" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="54" xr:uid="{00000000-000A-0000-FFFF-FFFF39000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
   <cacheFields count="6">
     <cacheField name="Date" numFmtId="14">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2020-03-02T00:00:00" maxDate="2020-04-25T00:00:00" count="11">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2020-03-02T00:00:00" maxDate="2020-04-28T00:00:00" count="12">
         <d v="2020-03-02T00:00:00"/>
         <d v="2020-03-11T00:00:00"/>
         <d v="2020-03-12T00:00:00"/>
@@ -1522,6 +1534,7 @@
         <d v="2020-04-20T00:00:00"/>
         <d v="2020-04-22T00:00:00"/>
         <d v="2020-04-24T00:00:00"/>
+        <d v="2020-04-27T00:00:00"/>
         <d v="2020-03-30T00:00:00" u="1"/>
         <d v="2020-03-26T00:00:00" u="1"/>
       </sharedItems>
@@ -1586,7 +1599,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="53">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="54">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -2011,26 +2024,35 @@
     <n v="0"/>
     <n v="0"/>
   </r>
+  <r>
+    <x v="9"/>
+    <x v="1"/>
+    <x v="11"/>
+    <n v="-1.5"/>
+    <n v="0"/>
+    <n v="1.5"/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="total" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="work-buckets" colHeaderCaption="date">
-  <location ref="A3:K26" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <location ref="A3:L26" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisCol" numFmtId="164" showAll="0">
-      <items count="12">
+      <items count="13">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
+        <item m="1" x="11"/>
         <item m="1" x="10"/>
-        <item m="1" x="9"/>
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
         <item x="6"/>
         <item x="7"/>
         <item x="8"/>
+        <item x="9"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2156,7 +2178,7 @@
   <colFields count="1">
     <field x="0"/>
   </colFields>
-  <colItems count="10">
+  <colItems count="11">
     <i>
       <x/>
     </i>
@@ -2183,6 +2205,9 @@
     </i>
     <i>
       <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
     </i>
     <i t="grand">
       <x/>
@@ -2334,21 +2359,22 @@
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:C12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <location ref="A3:C13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" numFmtId="14" showAll="0">
-      <items count="12">
+      <items count="13">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
+        <item m="1" x="11"/>
         <item m="1" x="10"/>
-        <item m="1" x="9"/>
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
         <item x="6"/>
         <item x="7"/>
         <item x="8"/>
+        <item x="9"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2361,7 +2387,7 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="9">
+  <rowItems count="10">
     <i>
       <x/>
     </i>
@@ -2388,6 +2414,9 @@
     </i>
     <i>
       <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
     </i>
   </rowItems>
   <colFields count="1">
@@ -2418,8 +2447,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F54" totalsRowShown="0">
-  <autoFilter ref="A1:F54" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F55" totalsRowShown="0">
+  <autoFilter ref="A1:F55" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="level-1"/>
@@ -2699,10 +2728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E57" sqref="E56:E57"/>
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3890,6 +3919,28 @@
         <v>0</v>
       </c>
     </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="6">
+        <v>43948</v>
+      </c>
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55">
+        <v>-1.5</v>
+      </c>
+      <c r="E55" s="5">
+        <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="F55" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>1.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3900,21 +3951,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A3:K26"/>
+  <dimension ref="A3:L26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>41</v>
       </c>
@@ -3922,7 +3973,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>42</v>
       </c>
@@ -3953,11 +4004,14 @@
       <c r="J4" s="9">
         <v>43945</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="K4" s="9">
+        <v>43948</v>
+      </c>
+      <c r="L4" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -3976,11 +4030,12 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K5" s="5"/>
+      <c r="L5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -4006,10 +4061,13 @@
         <v>0</v>
       </c>
       <c r="K6" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-1.5</v>
+      </c>
+      <c r="L6" s="5">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>12</v>
       </c>
@@ -4024,11 +4082,12 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
-      <c r="K7" s="5">
+      <c r="K7" s="5"/>
+      <c r="L7" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>14</v>
       </c>
@@ -4045,11 +4104,12 @@
         <v>-2</v>
       </c>
       <c r="J8" s="5"/>
-      <c r="K8" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K8" s="5"/>
+      <c r="L8" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>17</v>
       </c>
@@ -4071,10 +4131,13 @@
         <v>0</v>
       </c>
       <c r="K9" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-1.5</v>
+      </c>
+      <c r="L9" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>11</v>
       </c>
@@ -4091,11 +4154,12 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K10" s="5"/>
+      <c r="L10" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>10</v>
       </c>
@@ -4112,11 +4176,12 @@
         <v>-1</v>
       </c>
       <c r="J11" s="5"/>
-      <c r="K11" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K11" s="5"/>
+      <c r="L11" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>13</v>
       </c>
@@ -4133,11 +4198,12 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K12" s="5"/>
+      <c r="L12" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>16</v>
       </c>
@@ -4154,11 +4220,12 @@
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="5">
+      <c r="K13" s="5"/>
+      <c r="L13" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
@@ -4173,11 +4240,12 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="5">
+      <c r="K14" s="5"/>
+      <c r="L14" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
@@ -4196,11 +4264,12 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
-      <c r="K15" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K15" s="5"/>
+      <c r="L15" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>23</v>
       </c>
@@ -4219,11 +4288,12 @@
         <v>-1.5</v>
       </c>
       <c r="J16" s="5"/>
-      <c r="K16" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K16" s="5"/>
+      <c r="L16" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>27</v>
       </c>
@@ -4240,11 +4310,12 @@
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
-      <c r="K17" s="5">
+      <c r="K17" s="5"/>
+      <c r="L17" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>28</v>
       </c>
@@ -4259,11 +4330,12 @@
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
-      <c r="K18" s="5">
+      <c r="K18" s="5"/>
+      <c r="L18" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>29</v>
       </c>
@@ -4280,11 +4352,12 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
-      <c r="K19" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="5"/>
+      <c r="L19" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>30</v>
       </c>
@@ -4301,11 +4374,12 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
-      <c r="K20" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K20" s="5"/>
+      <c r="L20" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>31</v>
       </c>
@@ -4324,11 +4398,12 @@
         <v>-3</v>
       </c>
       <c r="J21" s="5"/>
-      <c r="K21" s="5">
+      <c r="K21" s="5"/>
+      <c r="L21" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>32</v>
       </c>
@@ -4345,11 +4420,12 @@
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
-      <c r="K22" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K22" s="5"/>
+      <c r="L22" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>33</v>
       </c>
@@ -4366,11 +4442,12 @@
         <v>-1</v>
       </c>
       <c r="J23" s="5"/>
-      <c r="K23" s="5">
+      <c r="K23" s="5"/>
+      <c r="L23" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>34</v>
       </c>
@@ -4387,11 +4464,12 @@
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
-      <c r="K24" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K24" s="5"/>
+      <c r="L24" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>40</v>
       </c>
@@ -4408,11 +4486,12 @@
         <v>-2</v>
       </c>
       <c r="J25" s="5"/>
-      <c r="K25" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K25" s="5"/>
+      <c r="L25" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>43</v>
       </c>
@@ -4444,7 +4523,10 @@
         <v>0</v>
       </c>
       <c r="K26" s="5">
-        <v>10</v>
+        <v>-1.5</v>
+      </c>
+      <c r="L26" s="5">
+        <v>8.5</v>
       </c>
     </row>
   </sheetData>
@@ -4454,10 +4536,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A3:H13"/>
+  <dimension ref="A3:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4698,10 +4780,33 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F13" s="7">
+      <c r="A13" s="3">
+        <v>43948</v>
+      </c>
+      <c r="B13" s="5">
+        <v>25.5</v>
+      </c>
+      <c r="C13" s="5">
+        <v>17</v>
+      </c>
+      <c r="F13" s="6">
+        <f t="shared" ref="F13" si="19">A13</f>
+        <v>43948</v>
+      </c>
+      <c r="G13">
+        <f t="shared" ref="G13" si="20">B13</f>
+        <v>25.5</v>
+      </c>
+      <c r="H13">
+        <f t="shared" ref="H13" si="21">C13</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F14" s="7">
         <v>44013</v>
       </c>
-      <c r="G13">
+      <c r="G14">
         <v>25.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated burnup/README for 4-29-2020 meeting
</commit_message>
<xml_diff>
--- a/misc/klask-burn-up.xlsx
+++ b/misc/klask-burn-up.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trevo\OneDrive\Documents\GitHub\klask\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1643E8-4396-4069-93FD-B8366C26591A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DF88E5-86C6-4461-B363-675046513A39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data-entry" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="50">
   <si>
     <t>Date</t>
   </si>
@@ -174,6 +174,21 @@
   <si>
     <t>booby-prize-most-klasks</t>
   </si>
+  <si>
+    <t>level-3</t>
+  </si>
+  <si>
+    <t>fix-hard-coding</t>
+  </si>
+  <si>
+    <t>(blank)</t>
+  </si>
+  <si>
+    <t>most-loc-points</t>
+  </si>
+  <si>
+    <t>most-biscuit-points</t>
+  </si>
 </sst>
 </file>
 
@@ -182,10 +197,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -223,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -246,11 +267,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="27">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -321,6 +345,20 @@
       <fill>
         <patternFill patternType="solid">
           <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -522,10 +560,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'burn-up'!$F$4:$F$14</c:f>
+              <c:f>'burn-up'!$F$4:$F$15</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>43892</c:v>
                 </c:pt>
@@ -556,7 +594,10 @@
                 <c:pt idx="9">
                   <c:v>43948</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="d\-mmm">
+                <c:pt idx="10">
+                  <c:v>43950</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="d\-mmm">
                   <c:v>44013</c:v>
                 </c:pt>
               </c:numCache>
@@ -564,10 +605,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'burn-up'!$G$4:$G$14</c:f>
+              <c:f>'burn-up'!$G$4:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>39.5</c:v>
                 </c:pt>
@@ -599,7 +640,10 @@
                   <c:v>25.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>25.5</c:v>
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>27.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -654,10 +698,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>'burn-up'!$F$4:$F$14</c:f>
+              <c:f>'burn-up'!$F$4:$F$15</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>43892</c:v>
                 </c:pt>
@@ -688,7 +732,10 @@
                 <c:pt idx="9">
                   <c:v>43948</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="d\-mmm">
+                <c:pt idx="10">
+                  <c:v>43950</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="d\-mmm">
                   <c:v>44013</c:v>
                 </c:pt>
               </c:numCache>
@@ -696,10 +743,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'burn-up'!$H$4:$H$13</c:f>
+              <c:f>'burn-up'!$H$4:$H$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -729,6 +776,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1480,16 +1530,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1483995</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>182880</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>173355</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>558165</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1518,13 +1568,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Trevor Moldenhauer" refreshedDate="43948.638872337964" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="54" xr:uid="{00000000-000A-0000-FFFF-FFFF39000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Trevor Moldenhauer" refreshedDate="43950.628449768519" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="60" xr:uid="{00000000-000A-0000-FFFF-FFFF39000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
-  <cacheFields count="6">
+  <cacheFields count="7">
     <cacheField name="Date" numFmtId="14">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2020-03-02T00:00:00" maxDate="2020-04-28T00:00:00" count="12">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2020-03-02T00:00:00" maxDate="2020-04-30T00:00:00" count="13">
         <d v="2020-03-02T00:00:00"/>
         <d v="2020-03-11T00:00:00"/>
         <d v="2020-03-12T00:00:00"/>
@@ -1535,8 +1585,9 @@
         <d v="2020-04-22T00:00:00"/>
         <d v="2020-04-24T00:00:00"/>
         <d v="2020-04-27T00:00:00"/>
+        <d v="2020-04-29T00:00:00"/>
+        <d v="2020-03-26T00:00:00" u="1"/>
         <d v="2020-03-30T00:00:00" u="1"/>
-        <d v="2020-03-26T00:00:00" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="level-1" numFmtId="0">
@@ -1550,7 +1601,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="level-2" numFmtId="0">
-      <sharedItems count="27">
+      <sharedItems count="29">
         <s v="ionic-info"/>
         <s v="mob-programming"/>
         <s v="research-bracket"/>
@@ -1577,7 +1628,15 @@
         <s v="css-aesthetics"/>
         <s v="tourney-recruiting"/>
         <s v="web-api"/>
+        <s v="most-loc-points"/>
+        <s v="most-biscuit-points"/>
         <s v="booby-prize" u="1"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="level-3" numFmtId="0">
+      <sharedItems containsBlank="1" count="2">
+        <m/>
+        <s v="fix-hard-coding"/>
       </sharedItems>
     </cacheField>
     <cacheField name="size-delta" numFmtId="0">
@@ -1599,8 +1658,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="54">
-  <r>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="60">
+  <r>
+    <x v="0"/>
     <x v="0"/>
     <x v="0"/>
     <x v="0"/>
@@ -1611,441 +1671,548 @@
   <r>
     <x v="0"/>
     <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <n v="0.5"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <n v="0.5"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="0"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="7"/>
+    <x v="0"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="8"/>
+    <x v="0"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="9"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="10"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="11"/>
+    <x v="0"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="12"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="13"/>
+    <x v="0"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="14"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="15"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <n v="0.5"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="16"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="17"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <n v="0.5"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="18"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="19"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="20"/>
+    <x v="0"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="21"/>
+    <x v="0"/>
+    <n v="1.5"/>
+    <n v="1.5"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="22"/>
+    <x v="0"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="23"/>
+    <x v="0"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="24"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <n v="0.5"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="-0.5"/>
+    <n v="0"/>
+    <n v="0.5"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="-3"/>
+    <n v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="-0.5"/>
+    <n v="0"/>
+    <n v="0.5"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="-0.5"/>
+    <n v="0"/>
+    <n v="0.5"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="-1"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="5"/>
+    <x v="22"/>
+    <x v="0"/>
+    <n v="-3"/>
+    <n v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="5"/>
+    <x v="25"/>
+    <x v="0"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="4"/>
+    <x v="20"/>
+    <x v="0"/>
+    <n v="-3"/>
+    <n v="-3"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="4"/>
+    <x v="21"/>
+    <x v="0"/>
+    <n v="-1.5"/>
+    <n v="-1.5"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="5"/>
+    <x v="24"/>
+    <x v="0"/>
+    <n v="-0.5"/>
+    <n v="-0.5"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="18"/>
+    <x v="0"/>
+    <n v="-1"/>
+    <n v="-1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="12"/>
+    <x v="0"/>
+    <n v="-1"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="15"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <n v="0.5"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="7"/>
+    <x v="0"/>
+    <n v="-2"/>
+    <n v="0"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="15"/>
+    <x v="0"/>
+    <n v="-1"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="13"/>
+    <x v="0"/>
+    <n v="-3"/>
+    <n v="-3"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="14"/>
+    <x v="0"/>
+    <n v="-1"/>
+    <n v="-1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="0"/>
+    <n v="-1"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="1"/>
+    <x v="10"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="1"/>
+    <x v="11"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="1"/>
+    <x v="11"/>
+    <x v="0"/>
+    <n v="-1"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="-1"/>
+    <n v="-1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="1"/>
+    <x v="8"/>
+    <x v="0"/>
+    <n v="-2"/>
+    <n v="-2"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="3"/>
+    <x v="16"/>
+    <x v="0"/>
+    <n v="-1"/>
+    <n v="-1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="3"/>
+    <x v="17"/>
+    <x v="0"/>
+    <n v="-0.5"/>
+    <n v="-0.5"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="5"/>
+    <x v="23"/>
+    <x v="0"/>
+    <n v="-1"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="5"/>
+    <x v="25"/>
+    <x v="0"/>
+    <n v="-2"/>
+    <n v="-2"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="1"/>
+    <x v="11"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="1"/>
+    <x v="11"/>
+    <x v="0"/>
+    <n v="-1.5"/>
+    <n v="0"/>
+    <n v="1.5"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="1"/>
+    <x v="11"/>
+    <x v="0"/>
+    <n v="-0.5"/>
+    <n v="0"/>
+    <n v="0.5"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="1"/>
+    <x v="9"/>
+    <x v="0"/>
+    <n v="-1"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="0"/>
+    <n v="-3"/>
+    <n v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="1"/>
+    <x v="11"/>
     <x v="1"/>
     <n v="0.5"/>
     <n v="0.5"/>
     <n v="0"/>
   </r>
   <r>
-    <x v="0"/>
-    <x v="0"/>
+    <x v="10"/>
     <x v="2"/>
-    <n v="0.5"/>
-    <n v="0.5"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="3"/>
-    <n v="4"/>
-    <n v="4"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="4"/>
-    <n v="1"/>
-    <n v="1"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="5"/>
-    <n v="1"/>
-    <n v="1"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="6"/>
-    <n v="3"/>
-    <n v="3"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="7"/>
-    <n v="2"/>
-    <n v="2"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="8"/>
-    <n v="2"/>
-    <n v="2"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="9"/>
-    <n v="1"/>
-    <n v="1"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
+    <x v="26"/>
+    <x v="0"/>
+    <n v="0.75"/>
+    <n v="0.75"/>
+    <n v="0"/>
+  </r>
+  <r>
     <x v="10"/>
-    <n v="1"/>
-    <n v="1"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="11"/>
-    <n v="3"/>
-    <n v="3"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
     <x v="2"/>
-    <x v="12"/>
-    <n v="1"/>
-    <n v="1"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="13"/>
-    <n v="3"/>
-    <n v="3"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="14"/>
-    <n v="1"/>
-    <n v="1"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="15"/>
-    <n v="0.5"/>
-    <n v="0.5"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="3"/>
-    <x v="16"/>
-    <n v="1"/>
-    <n v="1"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="3"/>
-    <x v="17"/>
-    <n v="0.5"/>
-    <n v="0.5"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="3"/>
-    <x v="18"/>
-    <n v="1"/>
-    <n v="1"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="4"/>
-    <x v="19"/>
-    <n v="1"/>
-    <n v="1"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="4"/>
-    <x v="20"/>
-    <n v="3"/>
-    <n v="3"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="4"/>
-    <x v="21"/>
-    <n v="1.5"/>
-    <n v="1.5"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="5"/>
-    <x v="22"/>
-    <n v="3"/>
-    <n v="3"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="5"/>
-    <x v="23"/>
-    <n v="3"/>
-    <n v="3"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="5"/>
-    <x v="24"/>
-    <n v="0.5"/>
-    <n v="0.5"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <n v="-0.5"/>
-    <n v="0"/>
-    <n v="0.5"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="3"/>
-    <n v="-3"/>
-    <n v="0"/>
-    <n v="3"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="-0.5"/>
-    <n v="0"/>
-    <n v="0.5"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="1"/>
-    <n v="-0.5"/>
-    <n v="0"/>
-    <n v="0.5"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="3"/>
-    <n v="-1"/>
-    <n v="0"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="5"/>
-    <x v="22"/>
-    <n v="-3"/>
-    <n v="0"/>
-    <n v="3"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="5"/>
-    <x v="25"/>
-    <n v="2"/>
-    <n v="2"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="20"/>
-    <n v="-3"/>
-    <n v="-3"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="21"/>
-    <n v="-1.5"/>
-    <n v="-1.5"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="5"/>
-    <x v="24"/>
-    <n v="-0.5"/>
-    <n v="-0.5"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-    <x v="18"/>
-    <n v="-1"/>
-    <n v="-1"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <x v="2"/>
-    <x v="12"/>
-    <n v="-1"/>
-    <n v="0"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <x v="2"/>
-    <x v="15"/>
-    <n v="0.5"/>
-    <n v="0.5"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <x v="1"/>
-    <x v="7"/>
-    <n v="-2"/>
-    <n v="0"/>
-    <n v="2"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <x v="2"/>
-    <x v="15"/>
-    <n v="-1"/>
-    <n v="0"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <x v="2"/>
-    <x v="13"/>
-    <n v="-3"/>
-    <n v="-3"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <x v="2"/>
-    <x v="14"/>
-    <n v="-1"/>
-    <n v="-1"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <x v="1"/>
-    <x v="5"/>
-    <n v="-1"/>
-    <n v="0"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="6"/>
-    <x v="1"/>
-    <x v="10"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="6"/>
-    <x v="1"/>
-    <x v="11"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <x v="1"/>
-    <x v="11"/>
-    <n v="-1"/>
-    <n v="0"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <x v="1"/>
-    <x v="4"/>
-    <n v="-1"/>
-    <n v="-1"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <x v="1"/>
-    <x v="8"/>
-    <n v="-2"/>
-    <n v="-2"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <x v="3"/>
-    <x v="16"/>
-    <n v="-1"/>
-    <n v="-1"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <x v="3"/>
-    <x v="17"/>
-    <n v="-0.5"/>
-    <n v="-0.5"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <x v="5"/>
-    <x v="23"/>
-    <n v="-1"/>
-    <n v="0"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <x v="5"/>
-    <x v="25"/>
-    <n v="-2"/>
-    <n v="-2"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="8"/>
-    <x v="1"/>
-    <x v="11"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <x v="9"/>
-    <x v="1"/>
-    <x v="11"/>
-    <n v="-1.5"/>
-    <n v="0"/>
-    <n v="1.5"/>
+    <x v="27"/>
+    <x v="0"/>
+    <n v="0.75"/>
+    <n v="0.75"/>
+    <n v="0"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="total" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="work-buckets" colHeaderCaption="date">
-  <location ref="A3:L26" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="6">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="total" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="work-buckets" colHeaderCaption="date">
+  <location ref="A3:M33" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="7">
     <pivotField axis="axisCol" numFmtId="164" showAll="0">
-      <items count="13">
+      <items count="14">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
         <item m="1" x="11"/>
-        <item m="1" x="10"/>
+        <item m="1" x="12"/>
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
@@ -2053,6 +2220,7 @@
         <item x="7"/>
         <item x="8"/>
         <item x="9"/>
+        <item x="10"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2060,31 +2228,31 @@
       <items count="7">
         <item sd="0" x="0"/>
         <item x="1"/>
-        <item sd="0" x="2"/>
+        <item x="2"/>
         <item sd="0" x="3"/>
-        <item x="4"/>
-        <item x="5"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisRow" showAll="0">
-      <items count="28">
-        <item x="6"/>
+      <items count="30">
+        <item sd="0" x="6"/>
         <item x="3"/>
-        <item x="8"/>
+        <item sd="0" x="8"/>
         <item x="11"/>
         <item x="0"/>
-        <item x="5"/>
+        <item sd="0" x="5"/>
         <item x="1"/>
-        <item x="4"/>
-        <item x="7"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="7"/>
         <item x="2"/>
-        <item x="10"/>
-        <item x="9"/>
+        <item sd="0" x="10"/>
+        <item sd="0" x="9"/>
         <item x="12"/>
         <item x="13"/>
         <item x="14"/>
-        <item m="1" x="26"/>
+        <item m="1" x="28"/>
         <item x="16"/>
         <item x="17"/>
         <item x="18"/>
@@ -2096,6 +2264,15 @@
         <item x="24"/>
         <item x="25"/>
         <item x="15"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2103,11 +2280,12 @@
     <pivotField showAll="0" defaultSubtotal="0"/>
     <pivotField showAll="0" defaultSubtotal="0"/>
   </pivotFields>
-  <rowFields count="2">
+  <rowFields count="3">
     <field x="1"/>
     <field x="2"/>
+    <field x="3"/>
   </rowFields>
-  <rowItems count="22">
+  <rowItems count="29">
     <i>
       <x/>
     </i>
@@ -2122,6 +2300,12 @@
     </i>
     <i r="1">
       <x v="3"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
     </i>
     <i r="1">
       <x v="5"/>
@@ -2141,35 +2325,50 @@
     <i>
       <x v="2"/>
     </i>
+    <i r="1">
+      <x v="12"/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="13"/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="14"/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="26"/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="27"/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="28"/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
     <i>
       <x v="3"/>
     </i>
     <i>
       <x v="4"/>
     </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i r="1">
-      <x v="20"/>
-    </i>
-    <i r="1">
-      <x v="21"/>
-    </i>
     <i>
       <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="22"/>
-    </i>
-    <i r="1">
-      <x v="23"/>
-    </i>
-    <i r="1">
-      <x v="24"/>
-    </i>
-    <i r="1">
-      <x v="25"/>
     </i>
     <i t="grand">
       <x/>
@@ -2178,7 +2377,7 @@
   <colFields count="1">
     <field x="0"/>
   </colFields>
-  <colItems count="11">
+  <colItems count="12">
     <i>
       <x/>
     </i>
@@ -2209,15 +2408,18 @@
     <i>
       <x v="11"/>
     </i>
+    <i>
+      <x v="12"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
   </colItems>
   <dataFields count="1">
-    <dataField name="backlog-breakdown" fld="3" baseField="0" baseItem="0"/>
+    <dataField name="backlog-breakdown" fld="4" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="11">
-    <format dxfId="21">
+  <formats count="12">
+    <format dxfId="23">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2226,6 +2428,25 @@
           <reference field="2" count="1">
             <x v="8"/>
           </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="22">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="2" count="1">
+            <x v="12"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="21">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
@@ -2242,25 +2463,6 @@
       </pivotArea>
     </format>
     <format dxfId="19">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="18">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="2">
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="2" count="1">
-            <x v="12"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="17">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2272,7 +2474,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2280,6 +2482,30 @@
           </reference>
           <reference field="2" count="1">
             <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="17">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="2" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="16">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="2" count="1">
+            <x v="26"/>
           </reference>
         </references>
       </pivotArea>
@@ -2300,10 +2526,10 @@
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
-            <x v="2"/>
+            <x v="1"/>
           </reference>
           <reference field="2" count="1">
-            <x v="26"/>
+            <x v="10"/>
           </reference>
         </references>
       </pivotArea>
@@ -2315,24 +2541,12 @@
             <x v="1"/>
           </reference>
           <reference field="2" count="1">
-            <x v="5"/>
+            <x v="3"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="12">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="2">
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="2" count="1">
-            <x v="10"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="11">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2358,16 +2572,16 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:C13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="6">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C14" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
     <pivotField axis="axisRow" numFmtId="14" showAll="0">
-      <items count="13">
+      <items count="14">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
         <item m="1" x="11"/>
-        <item m="1" x="10"/>
+        <item m="1" x="12"/>
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
@@ -2375,9 +2589,11 @@
         <item x="7"/>
         <item x="8"/>
         <item x="9"/>
+        <item x="10"/>
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -2387,7 +2603,7 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="10">
+  <rowItems count="11">
     <i>
       <x/>
     </i>
@@ -2418,6 +2634,9 @@
     <i>
       <x v="11"/>
     </i>
+    <i>
+      <x v="12"/>
+    </i>
   </rowItems>
   <colFields count="1">
     <field x="-2"/>
@@ -2431,8 +2650,8 @@
     </i>
   </colItems>
   <dataFields count="2">
-    <dataField name="Sum of release-target" fld="4" showDataAs="runTotal" baseField="0" baseItem="0"/>
-    <dataField name="Sum of work-completed" fld="5" showDataAs="runTotal" baseField="0" baseItem="0"/>
+    <dataField name="Sum of release-target" fld="5" showDataAs="runTotal" baseField="0" baseItem="0"/>
+    <dataField name="Sum of work-completed" fld="6" showDataAs="runTotal" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -2447,17 +2666,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F55" totalsRowShown="0">
-  <autoFilter ref="A1:F55" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G61" totalsRowShown="0">
+  <autoFilter ref="A1:G61" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="26"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="level-1"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="level-2"/>
+    <tableColumn id="7" xr3:uid="{2C6C122A-C642-4B3B-900D-A057FFF35EE9}" name="level-3"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="size-delta"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="release-target" dataDxfId="23">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="release-target" dataDxfId="25">
       <calculatedColumnFormula>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="work-completed" dataDxfId="22">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="work-completed" dataDxfId="24">
       <calculatedColumnFormula>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2728,10 +2948,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2739,12 +2959,12 @@
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2755,16 +2975,19 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>35</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43892</v>
       </c>
@@ -2774,19 +2997,19 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>0.5</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>0.5</v>
       </c>
-      <c r="F2">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43892</v>
       </c>
@@ -2796,19 +3019,19 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0.5</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>0.5</v>
       </c>
-      <c r="F3">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43892</v>
       </c>
@@ -2818,19 +3041,19 @@
       <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>0.5</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>0.5</v>
       </c>
-      <c r="F4">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43892</v>
       </c>
@@ -2840,19 +3063,19 @@
       <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>4</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>4</v>
       </c>
-      <c r="F5">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43892</v>
       </c>
@@ -2862,19 +3085,19 @@
       <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>1</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>1</v>
       </c>
-      <c r="F6">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43892</v>
       </c>
@@ -2884,19 +3107,19 @@
       <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>1</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>1</v>
       </c>
-      <c r="F7">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43892</v>
       </c>
@@ -2906,19 +3129,19 @@
       <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>3</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>3</v>
       </c>
-      <c r="F8">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43892</v>
       </c>
@@ -2928,19 +3151,19 @@
       <c r="C9" t="s">
         <v>13</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>2</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>2</v>
       </c>
-      <c r="F9">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43892</v>
       </c>
@@ -2950,19 +3173,19 @@
       <c r="C10" t="s">
         <v>14</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>2</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>2</v>
       </c>
-      <c r="F10">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43892</v>
       </c>
@@ -2972,19 +3195,19 @@
       <c r="C11" t="s">
         <v>15</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>1</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>1</v>
       </c>
-      <c r="F11">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43892</v>
       </c>
@@ -2994,19 +3217,19 @@
       <c r="C12" t="s">
         <v>16</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>1</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>1</v>
       </c>
-      <c r="F12">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43892</v>
       </c>
@@ -3016,19 +3239,19 @@
       <c r="C13" t="s">
         <v>17</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>3</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>3</v>
       </c>
-      <c r="F13">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43892</v>
       </c>
@@ -3038,19 +3261,19 @@
       <c r="C14" t="s">
         <v>20</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>1</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>1</v>
       </c>
-      <c r="F14">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43892</v>
       </c>
@@ -3060,19 +3283,19 @@
       <c r="C15" t="s">
         <v>21</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>3</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>3</v>
       </c>
-      <c r="F15">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43892</v>
       </c>
@@ -3082,19 +3305,19 @@
       <c r="C16" t="s">
         <v>22</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>1</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>1</v>
       </c>
-      <c r="F16">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43892</v>
       </c>
@@ -3104,19 +3327,19 @@
       <c r="C17" t="s">
         <v>44</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>0.5</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>0.5</v>
       </c>
-      <c r="F17">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43892</v>
       </c>
@@ -3126,19 +3349,19 @@
       <c r="C18" t="s">
         <v>24</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>1</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>1</v>
       </c>
-      <c r="F18">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43892</v>
       </c>
@@ -3148,19 +3371,19 @@
       <c r="C19" t="s">
         <v>25</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>0.5</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>0.5</v>
       </c>
-      <c r="F19">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43892</v>
       </c>
@@ -3170,19 +3393,19 @@
       <c r="C20" t="s">
         <v>26</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>1</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>1</v>
       </c>
-      <c r="F20">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43892</v>
       </c>
@@ -3192,19 +3415,19 @@
       <c r="C21" t="s">
         <v>28</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>1</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>1</v>
       </c>
-      <c r="F21">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43892</v>
       </c>
@@ -3214,19 +3437,19 @@
       <c r="C22" t="s">
         <v>29</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>3</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>3</v>
       </c>
-      <c r="F22">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43892</v>
       </c>
@@ -3236,19 +3459,19 @@
       <c r="C23" t="s">
         <v>30</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>1.5</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>1.5</v>
       </c>
-      <c r="F23">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43892</v>
       </c>
@@ -3258,19 +3481,19 @@
       <c r="C24" t="s">
         <v>32</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>3</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>3</v>
       </c>
-      <c r="F24">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43892</v>
       </c>
@@ -3280,19 +3503,19 @@
       <c r="C25" t="s">
         <v>33</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>3</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>3</v>
       </c>
-      <c r="F25">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43892</v>
       </c>
@@ -3302,19 +3525,19 @@
       <c r="C26" t="s">
         <v>34</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>0.5</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>0.5</v>
       </c>
-      <c r="F26">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43901</v>
       </c>
@@ -3324,19 +3547,19 @@
       <c r="C27" t="s">
         <v>7</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>-0.5</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>0</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43901</v>
       </c>
@@ -3346,19 +3569,19 @@
       <c r="C28" t="s">
         <v>8</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>-3</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>0</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43902</v>
       </c>
@@ -3368,19 +3591,19 @@
       <c r="C29" t="s">
         <v>5</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>-0.5</v>
       </c>
-      <c r="E29" s="5">
+      <c r="F29" s="5">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>0</v>
       </c>
-      <c r="F29" s="5">
+      <c r="G29" s="5">
         <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43902</v>
       </c>
@@ -3390,19 +3613,19 @@
       <c r="C30" t="s">
         <v>6</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>-0.5</v>
       </c>
-      <c r="E30" s="5">
+      <c r="F30" s="5">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>0</v>
       </c>
-      <c r="F30" s="5">
+      <c r="G30" s="5">
         <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>43902</v>
       </c>
@@ -3412,19 +3635,19 @@
       <c r="C31" t="s">
         <v>8</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>-1</v>
       </c>
-      <c r="E31" s="5">
+      <c r="F31" s="5">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>0</v>
       </c>
-      <c r="F31" s="5">
+      <c r="G31" s="5">
         <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>43934</v>
       </c>
@@ -3434,19 +3657,19 @@
       <c r="C32" t="s">
         <v>32</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>-3</v>
       </c>
-      <c r="E32" s="5">
+      <c r="F32" s="5">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>0</v>
       </c>
-      <c r="F32" s="5">
+      <c r="G32" s="5">
         <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>43934</v>
       </c>
@@ -3456,19 +3679,19 @@
       <c r="C33" t="s">
         <v>40</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>2</v>
       </c>
-      <c r="E33" s="5">
+      <c r="F33" s="5">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>2</v>
       </c>
-      <c r="F33" s="5">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>43934</v>
       </c>
@@ -3478,18 +3701,18 @@
       <c r="C34" t="s">
         <v>29</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>-3</v>
       </c>
-      <c r="E34" s="5">
+      <c r="F34" s="5">
         <v>-3</v>
       </c>
-      <c r="F34" s="5">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>43934</v>
       </c>
@@ -3499,18 +3722,18 @@
       <c r="C35" t="s">
         <v>30</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>-1.5</v>
       </c>
-      <c r="E35" s="5">
+      <c r="F35" s="5">
         <v>-1.5</v>
       </c>
-      <c r="F35" s="5">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>43934</v>
       </c>
@@ -3520,18 +3743,18 @@
       <c r="C36" t="s">
         <v>34</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>-0.5</v>
       </c>
-      <c r="E36" s="5">
+      <c r="F36" s="5">
         <v>-0.5</v>
       </c>
-      <c r="F36" s="5">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>43934</v>
       </c>
@@ -3541,18 +3764,18 @@
       <c r="C37" t="s">
         <v>26</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>-1</v>
       </c>
-      <c r="E37" s="5">
+      <c r="F37" s="5">
         <v>-1</v>
       </c>
-      <c r="F37" s="5">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>43936</v>
       </c>
@@ -3562,19 +3785,19 @@
       <c r="C38" t="s">
         <v>20</v>
       </c>
-      <c r="D38">
+      <c r="E38">
         <v>-1</v>
       </c>
-      <c r="E38" s="5">
+      <c r="F38" s="5">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>0</v>
       </c>
-      <c r="F38" s="5">
+      <c r="G38" s="5">
         <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>43936</v>
       </c>
@@ -3584,19 +3807,19 @@
       <c r="C39" t="s">
         <v>44</v>
       </c>
-      <c r="D39">
+      <c r="E39">
         <v>0.5</v>
       </c>
-      <c r="E39" s="5">
+      <c r="F39" s="5">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>0.5</v>
       </c>
-      <c r="F39" s="5">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>43936</v>
       </c>
@@ -3606,19 +3829,19 @@
       <c r="C40" t="s">
         <v>13</v>
       </c>
-      <c r="D40">
+      <c r="E40">
         <v>-2</v>
       </c>
-      <c r="E40" s="5">
+      <c r="F40" s="5">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>0</v>
       </c>
-      <c r="F40" s="5">
+      <c r="G40" s="5">
         <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>43938</v>
       </c>
@@ -3628,19 +3851,19 @@
       <c r="C41" t="s">
         <v>44</v>
       </c>
-      <c r="D41">
+      <c r="E41">
         <v>-1</v>
       </c>
-      <c r="E41" s="5">
+      <c r="F41" s="5">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>0</v>
       </c>
-      <c r="F41" s="5">
+      <c r="G41" s="5">
         <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>43938</v>
       </c>
@@ -3650,18 +3873,18 @@
       <c r="C42" t="s">
         <v>21</v>
       </c>
-      <c r="D42">
+      <c r="E42">
         <v>-3</v>
       </c>
-      <c r="E42" s="5">
+      <c r="F42" s="5">
         <v>-3</v>
       </c>
-      <c r="F42" s="5">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>43938</v>
       </c>
@@ -3671,18 +3894,18 @@
       <c r="C43" t="s">
         <v>22</v>
       </c>
-      <c r="D43">
+      <c r="E43">
         <v>-1</v>
       </c>
-      <c r="E43" s="5">
+      <c r="F43" s="5">
         <v>-1</v>
       </c>
-      <c r="F43" s="5">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>43938</v>
       </c>
@@ -3692,19 +3915,19 @@
       <c r="C44" t="s">
         <v>11</v>
       </c>
-      <c r="D44">
+      <c r="E44">
         <v>-1</v>
       </c>
-      <c r="E44" s="5">
+      <c r="F44" s="5">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>0</v>
       </c>
-      <c r="F44" s="5">
+      <c r="G44" s="5">
         <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>43941</v>
       </c>
@@ -3714,19 +3937,19 @@
       <c r="C45" t="s">
         <v>16</v>
       </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-      <c r="E45" s="5">
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45" s="5">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>0</v>
       </c>
-      <c r="F45" s="5">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>43941</v>
       </c>
@@ -3736,19 +3959,19 @@
       <c r="C46" t="s">
         <v>17</v>
       </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46" s="5">
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46" s="5">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>0</v>
       </c>
-      <c r="F46" s="5">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>43943</v>
       </c>
@@ -3758,19 +3981,19 @@
       <c r="C47" t="s">
         <v>17</v>
       </c>
-      <c r="D47">
+      <c r="E47">
         <v>-1</v>
       </c>
-      <c r="E47" s="5">
+      <c r="F47" s="5">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>0</v>
       </c>
-      <c r="F47" s="5">
+      <c r="G47" s="5">
         <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>43943</v>
       </c>
@@ -3780,18 +4003,18 @@
       <c r="C48" t="s">
         <v>10</v>
       </c>
-      <c r="D48">
+      <c r="E48">
         <v>-1</v>
       </c>
-      <c r="E48" s="5">
+      <c r="F48" s="5">
         <v>-1</v>
       </c>
-      <c r="F48" s="5">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>43943</v>
       </c>
@@ -3801,18 +4024,18 @@
       <c r="C49" t="s">
         <v>14</v>
       </c>
-      <c r="D49">
+      <c r="E49">
         <v>-2</v>
       </c>
-      <c r="E49" s="5">
+      <c r="F49" s="5">
         <v>-2</v>
       </c>
-      <c r="F49" s="5">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <v>43943</v>
       </c>
@@ -3822,18 +4045,18 @@
       <c r="C50" t="s">
         <v>24</v>
       </c>
-      <c r="D50">
+      <c r="E50">
         <v>-1</v>
       </c>
-      <c r="E50" s="5">
+      <c r="F50" s="5">
         <v>-1</v>
       </c>
-      <c r="F50" s="5">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
         <v>43943</v>
       </c>
@@ -3843,18 +4066,18 @@
       <c r="C51" t="s">
         <v>25</v>
       </c>
-      <c r="D51">
+      <c r="E51">
         <v>-0.5</v>
       </c>
-      <c r="E51" s="5">
+      <c r="F51" s="5">
         <v>-0.5</v>
       </c>
-      <c r="F51" s="5">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G51" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="6">
         <v>43943</v>
       </c>
@@ -3864,19 +4087,19 @@
       <c r="C52" t="s">
         <v>33</v>
       </c>
-      <c r="D52">
+      <c r="E52">
         <v>-1</v>
       </c>
-      <c r="E52" s="5">
+      <c r="F52" s="5">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>0</v>
       </c>
-      <c r="F52" s="5">
+      <c r="G52" s="5">
         <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="6">
         <v>43943</v>
       </c>
@@ -3886,18 +4109,18 @@
       <c r="C53" t="s">
         <v>40</v>
       </c>
-      <c r="D53">
+      <c r="E53">
         <v>-2</v>
       </c>
-      <c r="E53" s="5">
+      <c r="F53" s="5">
         <v>-2</v>
       </c>
-      <c r="F53" s="5">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G53" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
         <v>43945</v>
       </c>
@@ -3907,19 +4130,19 @@
       <c r="C54" t="s">
         <v>17</v>
       </c>
-      <c r="D54">
-        <v>0</v>
-      </c>
-      <c r="E54" s="5">
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54" s="5">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>0</v>
       </c>
-      <c r="F54" s="5">
-        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G54" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
         <v>43948</v>
       </c>
@@ -3929,19 +4152,155 @@
       <c r="C55" t="s">
         <v>17</v>
       </c>
-      <c r="D55">
+      <c r="E55">
         <v>-1.5</v>
       </c>
-      <c r="E55" s="5">
+      <c r="F55" s="5">
         <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
         <v>0</v>
       </c>
-      <c r="F55" s="5">
+      <c r="G55" s="5">
         <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
         <v>1.5</v>
       </c>
     </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="6">
+        <v>43950</v>
+      </c>
+      <c r="B56" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E56">
+        <v>-0.5</v>
+      </c>
+      <c r="F56" s="5">
+        <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G56" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="6">
+        <v>43950</v>
+      </c>
+      <c r="B57" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57" t="s">
+        <v>15</v>
+      </c>
+      <c r="E57">
+        <v>-1</v>
+      </c>
+      <c r="F57" s="5">
+        <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G57" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="6">
+        <v>43950</v>
+      </c>
+      <c r="B58" t="s">
+        <v>9</v>
+      </c>
+      <c r="C58" t="s">
+        <v>12</v>
+      </c>
+      <c r="E58">
+        <v>-3</v>
+      </c>
+      <c r="F58" s="5">
+        <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G58" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="6">
+        <v>43950</v>
+      </c>
+      <c r="B59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59" t="s">
+        <v>17</v>
+      </c>
+      <c r="D59" t="s">
+        <v>46</v>
+      </c>
+      <c r="E59">
+        <v>0.5</v>
+      </c>
+      <c r="F59" s="5">
+        <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G59" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="6">
+        <v>43950</v>
+      </c>
+      <c r="B60" t="s">
+        <v>19</v>
+      </c>
+      <c r="C60" t="s">
+        <v>48</v>
+      </c>
+      <c r="E60">
+        <v>0.75</v>
+      </c>
+      <c r="F60" s="5">
+        <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
+        <v>0.75</v>
+      </c>
+      <c r="G60" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="6">
+        <v>43950</v>
+      </c>
+      <c r="B61" t="s">
+        <v>19</v>
+      </c>
+      <c r="C61" t="s">
+        <v>49</v>
+      </c>
+      <c r="E61">
+        <v>0.75</v>
+      </c>
+      <c r="F61" s="5">
+        <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
+        <v>0.75</v>
+      </c>
+      <c r="G61" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -3951,21 +4310,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A3:L26"/>
+  <dimension ref="A3:M33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="11" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>41</v>
       </c>
@@ -3973,7 +4333,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>42</v>
       </c>
@@ -4007,11 +4367,14 @@
       <c r="K4" s="9">
         <v>43948</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="L4" s="9">
+        <v>43950</v>
+      </c>
+      <c r="M4" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -4031,11 +4394,12 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
-      <c r="L5" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L5" s="5"/>
+      <c r="M5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -4064,10 +4428,13 @@
         <v>-1.5</v>
       </c>
       <c r="L6" s="5">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>-4</v>
+      </c>
+      <c r="M6" s="5">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>12</v>
       </c>
@@ -4084,10 +4451,13 @@
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>-3</v>
+      </c>
+      <c r="M7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>14</v>
       </c>
@@ -4105,12 +4475,13 @@
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
-      <c r="L8" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="L8" s="5"/>
+      <c r="M8" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="5">
@@ -4134,78 +4505,90 @@
         <v>-1.5</v>
       </c>
       <c r="L9" s="5">
+        <v>0</v>
+      </c>
+      <c r="M9" s="5">
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="5">
-        <v>1</v>
-      </c>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="5">
-        <v>-1</v>
-      </c>
+      <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>10</v>
+        <v>0.5</v>
+      </c>
+      <c r="M10" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>47</v>
       </c>
       <c r="B11" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
+      <c r="H11" s="5">
+        <v>0</v>
+      </c>
       <c r="I11" s="5">
         <v>-1</v>
       </c>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
+      <c r="J11" s="5">
+        <v>0</v>
+      </c>
+      <c r="K11" s="5">
+        <v>-1.5</v>
+      </c>
       <c r="L11" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>-0.5</v>
+      </c>
+      <c r="M11" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="5">
-        <v>-2</v>
-      </c>
-      <c r="G12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5">
+        <v>-1</v>
+      </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
-      <c r="L12" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>16</v>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="B13" s="5">
         <v>1</v>
@@ -4215,109 +4598,116 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="5">
-        <v>0</v>
-      </c>
-      <c r="I13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5">
+        <v>-1</v>
+      </c>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
-      <c r="L13" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>15</v>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="B14" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+      <c r="F14" s="5">
+        <v>-2</v>
+      </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
-      <c r="L14" s="5">
+      <c r="L14" s="5"/>
+      <c r="M14" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="5">
         <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="5">
-        <v>5.5</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="5">
-        <v>-0.5</v>
-      </c>
-      <c r="G15" s="5">
-        <v>-5</v>
-      </c>
-      <c r="H15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5">
+        <v>0</v>
+      </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
-      <c r="L15" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>23</v>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="B16" s="5">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="5">
-        <v>-1</v>
-      </c>
+      <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
-      <c r="I16" s="5">
-        <v>-1.5</v>
-      </c>
+      <c r="I16" s="5"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <v>-1</v>
+      </c>
+      <c r="M16" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B17" s="5">
         <v>5.5</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="5">
-        <v>-4.5</v>
-      </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5">
+        <v>-0.5</v>
+      </c>
+      <c r="G17" s="5">
+        <v>-5</v>
+      </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>28</v>
+        <v>1.5</v>
+      </c>
+      <c r="M17" s="5">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>20</v>
       </c>
       <c r="B18" s="5">
         <v>1</v>
@@ -4325,208 +4715,380 @@
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+      <c r="F18" s="5">
+        <v>-1</v>
+      </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
-      <c r="L18" s="5">
+      <c r="L18" s="5"/>
+      <c r="M18" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="5">
         <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="5">
-        <v>3</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="5">
-        <v>-3</v>
-      </c>
-      <c r="F19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5">
+        <v>-1</v>
+      </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
-      <c r="L19" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L19" s="5"/>
+      <c r="M19" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B20" s="5">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
-      <c r="E20" s="5">
-        <v>-1.5</v>
-      </c>
+      <c r="E20" s="5"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
+      <c r="G20" s="5">
+        <v>-3</v>
+      </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
-      <c r="L20" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>31</v>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>47</v>
       </c>
       <c r="B21" s="5">
-        <v>6.5</v>
+        <v>3</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="5">
-        <v>-1.5</v>
-      </c>
+      <c r="E21" s="5"/>
       <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
+      <c r="G21" s="5">
+        <v>-3</v>
+      </c>
       <c r="H21" s="5"/>
-      <c r="I21" s="5">
-        <v>-3</v>
-      </c>
+      <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
-      <c r="L21" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L21" s="5"/>
+      <c r="M21" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B22" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
-      <c r="E22" s="5">
-        <v>-3</v>
-      </c>
+      <c r="E22" s="5"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
+      <c r="G22" s="5">
+        <v>-1</v>
+      </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>33</v>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>47</v>
       </c>
       <c r="B23" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+      <c r="G23" s="5">
+        <v>-1</v>
+      </c>
       <c r="H23" s="5"/>
-      <c r="I23" s="5">
-        <v>-1</v>
-      </c>
+      <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
-      <c r="L23" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>34</v>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="B24" s="5">
         <v>0.5</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="5">
-        <v>-0.5</v>
-      </c>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="G24" s="5">
+        <v>-1</v>
+      </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
-      <c r="L24" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="5">
+        <v>0.5</v>
+      </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
-      <c r="E25" s="5">
-        <v>2</v>
-      </c>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="G25" s="5">
+        <v>-1</v>
+      </c>
       <c r="H25" s="5"/>
-      <c r="I25" s="5">
-        <v>-2</v>
-      </c>
+      <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
-      <c r="L25" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="L25" s="5"/>
+      <c r="M25" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="M26" s="5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="M27" s="5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="M28" s="5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="M29" s="5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5">
+        <v>-1.5</v>
+      </c>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="5">
+        <v>5.5</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5">
+        <v>-4.5</v>
+      </c>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="5">
+        <v>6.5</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5">
+        <v>-1.5</v>
+      </c>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5">
+        <v>-3</v>
+      </c>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B33" s="5">
         <v>39.5</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C33" s="5">
         <v>-3.5</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D33" s="5">
         <v>-2</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E33" s="5">
         <v>-7</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F33" s="5">
         <v>-2.5</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G33" s="5">
         <v>-6</v>
       </c>
-      <c r="H26" s="5">
-        <v>0</v>
-      </c>
-      <c r="I26" s="5">
+      <c r="H33" s="5">
+        <v>0</v>
+      </c>
+      <c r="I33" s="5">
         <v>-8.5</v>
       </c>
-      <c r="J26" s="5">
-        <v>0</v>
-      </c>
-      <c r="K26" s="5">
+      <c r="J33" s="5">
+        <v>0</v>
+      </c>
+      <c r="K33" s="5">
         <v>-1.5</v>
       </c>
-      <c r="L26" s="5">
-        <v>8.5</v>
+      <c r="L33" s="5">
+        <v>-2.5</v>
+      </c>
+      <c r="M33" s="5">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -4536,10 +5098,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A3:H14"/>
+  <dimension ref="A3:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4803,11 +5365,34 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F14" s="7">
+      <c r="A14" s="3">
+        <v>43950</v>
+      </c>
+      <c r="B14" s="5">
+        <v>27.5</v>
+      </c>
+      <c r="C14" s="5">
+        <v>21.5</v>
+      </c>
+      <c r="F14" s="6">
+        <f t="shared" ref="F14" si="22">A14</f>
+        <v>43950</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ref="G14" si="23">B14</f>
+        <v>27.5</v>
+      </c>
+      <c r="H14">
+        <f t="shared" ref="H14" si="24">C14</f>
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F15" s="7">
         <v>44013</v>
       </c>
-      <c r="G14">
-        <v>25.5</v>
+      <c r="G15">
+        <v>27.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates burn-up chart and readme file
</commit_message>
<xml_diff>
--- a/misc/klask-burn-up.xlsx
+++ b/misc/klask-burn-up.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trevo\OneDrive\Documents\GitHub\klask\misc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valer\Documents\GitHub\klask\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DF88E5-86C6-4461-B363-675046513A39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F48908-E863-428D-A6C3-11FA3AB5C6C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data-entry" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="24" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="52">
   <si>
     <t>Date</t>
   </si>
@@ -189,6 +189,12 @@
   <si>
     <t>most-biscuit-points</t>
   </si>
+  <si>
+    <t>clean-up</t>
+  </si>
+  <si>
+    <t>klask-page-rename</t>
+  </si>
 </sst>
 </file>
 
@@ -274,7 +280,1127 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="195">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d;@"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d;@"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d;@"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d;@"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d;@"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d;@"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d;@"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d;@"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d;@"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d;@"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d;@"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d;@"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d;@"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d;@"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -522,7 +1648,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -560,10 +1686,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'burn-up'!$F$4:$F$15</c:f>
+              <c:f>'burn-up'!$F$4:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>43892</c:v>
                 </c:pt>
@@ -597,7 +1723,10 @@
                 <c:pt idx="10">
                   <c:v>43950</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="d\-mmm">
+                <c:pt idx="11">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="d\-mmm">
                   <c:v>44013</c:v>
                 </c:pt>
               </c:numCache>
@@ -605,10 +1734,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'burn-up'!$G$4:$G$15</c:f>
+              <c:f>'burn-up'!$G$4:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>39.5</c:v>
                 </c:pt>
@@ -643,7 +1772,10 @@
                   <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>27.5</c:v>
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -698,10 +1830,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>'burn-up'!$F$4:$F$15</c:f>
+              <c:f>'burn-up'!$F$4:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>43892</c:v>
                 </c:pt>
@@ -735,7 +1867,10 @@
                 <c:pt idx="10">
                   <c:v>43950</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="d\-mmm">
+                <c:pt idx="11">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="d\-mmm">
                   <c:v>44013</c:v>
                 </c:pt>
               </c:numCache>
@@ -743,10 +1878,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'burn-up'!$H$4:$H$14</c:f>
+              <c:f>'burn-up'!$H$4:$H$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -779,6 +1914,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -858,7 +1996,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="472556976"/>
@@ -918,7 +2056,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="472557808"/>
@@ -959,7 +2097,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1530,16 +2668,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>160020</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>173355</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>167640</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>74295</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1568,13 +2706,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Trevor Moldenhauer" refreshedDate="43950.628449768519" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="60" xr:uid="{00000000-000A-0000-FFFF-FFFF39000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Valeria Welsh" refreshedDate="43952.631736342591" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="66" xr:uid="{00000000-000A-0000-FFFF-FFFF39000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
   <cacheFields count="7">
     <cacheField name="Date" numFmtId="14">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2020-03-02T00:00:00" maxDate="2020-04-30T00:00:00" count="13">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2020-03-02T00:00:00" maxDate="2020-05-02T00:00:00" count="14">
         <d v="2020-03-02T00:00:00"/>
         <d v="2020-03-11T00:00:00"/>
         <d v="2020-03-12T00:00:00"/>
@@ -1586,6 +2724,7 @@
         <d v="2020-04-24T00:00:00"/>
         <d v="2020-04-27T00:00:00"/>
         <d v="2020-04-29T00:00:00"/>
+        <d v="2020-05-01T00:00:00"/>
         <d v="2020-03-26T00:00:00" u="1"/>
         <d v="2020-03-30T00:00:00" u="1"/>
       </sharedItems>
@@ -1601,7 +2740,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="level-2" numFmtId="0">
-      <sharedItems count="29">
+      <sharedItems count="31">
         <s v="ionic-info"/>
         <s v="mob-programming"/>
         <s v="research-bracket"/>
@@ -1630,6 +2769,8 @@
         <s v="web-api"/>
         <s v="most-loc-points"/>
         <s v="most-biscuit-points"/>
+        <s v="clean-up"/>
+        <s v="klask-page-rename"/>
         <s v="booby-prize" u="1"/>
       </sharedItems>
     </cacheField>
@@ -1658,7 +2799,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="60">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="66">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -2199,20 +3340,74 @@
     <n v="0.75"/>
     <n v="0"/>
   </r>
+  <r>
+    <x v="11"/>
+    <x v="1"/>
+    <x v="11"/>
+    <x v="1"/>
+    <n v="-0.5"/>
+    <n v="0"/>
+    <n v="0.5"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="2"/>
+    <x v="26"/>
+    <x v="0"/>
+    <n v="-0.75"/>
+    <n v="0"/>
+    <n v="0.75"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="2"/>
+    <x v="27"/>
+    <x v="0"/>
+    <n v="-0.75"/>
+    <n v="0"/>
+    <n v="0.75"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="2"/>
+    <x v="28"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <n v="0.5"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="4"/>
+    <x v="19"/>
+    <x v="0"/>
+    <n v="-0.5"/>
+    <n v="-0.5"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="2"/>
+    <x v="29"/>
+    <x v="0"/>
+    <n v="0.5"/>
+    <n v="0.5"/>
+    <n v="0"/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="total" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="work-buckets" colHeaderCaption="date">
-  <location ref="A3:M33" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="total" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="work-buckets" colHeaderCaption="date">
+  <location ref="A3:N33" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisCol" numFmtId="164" showAll="0">
-      <items count="14">
+      <items count="15">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
-        <item m="1" x="11"/>
         <item m="1" x="12"/>
+        <item m="1" x="13"/>
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
@@ -2221,6 +3416,7 @@
         <item x="8"/>
         <item x="9"/>
         <item x="10"/>
+        <item x="11"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2230,13 +3426,13 @@
         <item x="1"/>
         <item x="2"/>
         <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
+        <item x="4"/>
         <item sd="0" x="5"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisRow" showAll="0">
-      <items count="30">
+      <items count="32">
         <item sd="0" x="6"/>
         <item x="3"/>
         <item sd="0" x="8"/>
@@ -2249,23 +3445,25 @@
         <item x="2"/>
         <item sd="0" x="10"/>
         <item sd="0" x="9"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item m="1" x="28"/>
+        <item sd="0" x="12"/>
+        <item sd="0" x="13"/>
+        <item sd="0" x="14"/>
+        <item m="1" x="30"/>
         <item x="16"/>
         <item x="17"/>
         <item x="18"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
+        <item sd="0" x="19"/>
+        <item sd="0" x="20"/>
+        <item sd="0" x="21"/>
         <item x="22"/>
         <item x="23"/>
         <item x="24"/>
         <item x="25"/>
-        <item x="15"/>
-        <item x="26"/>
-        <item x="27"/>
+        <item sd="0" x="15"/>
+        <item sd="0" x="26"/>
+        <item sd="0" x="27"/>
+        <item sd="0" x="28"/>
+        <item x="29"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2328,35 +3526,26 @@
     <i r="1">
       <x v="12"/>
     </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
     <i r="1">
       <x v="13"/>
-    </i>
-    <i r="2">
-      <x v="1"/>
     </i>
     <i r="1">
       <x v="14"/>
     </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
     <i r="1">
       <x v="26"/>
-    </i>
-    <i r="2">
-      <x v="1"/>
     </i>
     <i r="1">
       <x v="27"/>
     </i>
-    <i r="2">
-      <x v="1"/>
+    <i r="1">
+      <x v="28"/>
     </i>
     <i r="1">
-      <x v="28"/>
+      <x v="29"/>
+    </i>
+    <i r="1">
+      <x v="30"/>
     </i>
     <i r="2">
       <x v="1"/>
@@ -2366,6 +3555,15 @@
     </i>
     <i>
       <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i r="1">
+      <x v="20"/>
+    </i>
+    <i r="1">
+      <x v="21"/>
     </i>
     <i>
       <x v="5"/>
@@ -2377,7 +3575,7 @@
   <colFields count="1">
     <field x="0"/>
   </colFields>
-  <colItems count="12">
+  <colItems count="13">
     <i>
       <x/>
     </i>
@@ -2411,6 +3609,9 @@
     <i>
       <x v="12"/>
     </i>
+    <i>
+      <x v="13"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
@@ -2419,7 +3620,7 @@
     <dataField name="backlog-breakdown" fld="4" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="12">
-    <format dxfId="23">
+    <format dxfId="191">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2431,7 +3632,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="22">
+    <format dxfId="190">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2443,14 +3644,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="21">
+    <format dxfId="189">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="20">
+    <format dxfId="188">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2462,7 +3663,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="19">
+    <format dxfId="187">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2474,7 +3675,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="18">
+    <format dxfId="186">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2486,7 +3687,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="17">
+    <format dxfId="185">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2498,7 +3699,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="184">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2510,7 +3711,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="15">
+    <format dxfId="183">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2522,7 +3723,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="14">
+    <format dxfId="182">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2534,7 +3735,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="181">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2546,7 +3747,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="12">
+    <format dxfId="180">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -2572,16 +3773,16 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:C14" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable3" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C15" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" numFmtId="14" showAll="0">
-      <items count="14">
+      <items count="15">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
-        <item m="1" x="11"/>
         <item m="1" x="12"/>
+        <item m="1" x="13"/>
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
@@ -2590,6 +3791,7 @@
         <item x="8"/>
         <item x="9"/>
         <item x="10"/>
+        <item x="11"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2603,7 +3805,7 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="11">
+  <rowItems count="12">
     <i>
       <x/>
     </i>
@@ -2637,6 +3839,9 @@
     <i>
       <x v="12"/>
     </i>
+    <i>
+      <x v="13"/>
+    </i>
   </rowItems>
   <colFields count="1">
     <field x="-2"/>
@@ -2666,18 +3871,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G61" totalsRowShown="0">
-  <autoFilter ref="A1:G61" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G67" totalsRowShown="0">
+  <autoFilter ref="A1:G67" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="194"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="level-1"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="level-2"/>
     <tableColumn id="7" xr3:uid="{2C6C122A-C642-4B3B-900D-A057FFF35EE9}" name="level-3"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="size-delta"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="release-target" dataDxfId="25">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="release-target" dataDxfId="193">
       <calculatedColumnFormula>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="work-completed" dataDxfId="24">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="work-completed" dataDxfId="192">
       <calculatedColumnFormula>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2948,23 +4153,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2987,7 +4192,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43892</v>
       </c>
@@ -3009,7 +4214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43892</v>
       </c>
@@ -3031,7 +4236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>43892</v>
       </c>
@@ -3053,7 +4258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>43892</v>
       </c>
@@ -3075,7 +4280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>43892</v>
       </c>
@@ -3097,7 +4302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>43892</v>
       </c>
@@ -3119,7 +4324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>43892</v>
       </c>
@@ -3141,7 +4346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>43892</v>
       </c>
@@ -3163,7 +4368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>43892</v>
       </c>
@@ -3185,7 +4390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>43892</v>
       </c>
@@ -3207,7 +4412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>43892</v>
       </c>
@@ -3229,7 +4434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>43892</v>
       </c>
@@ -3251,7 +4456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>43892</v>
       </c>
@@ -3273,7 +4478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>43892</v>
       </c>
@@ -3295,7 +4500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>43892</v>
       </c>
@@ -3317,7 +4522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>43892</v>
       </c>
@@ -3339,7 +4544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>43892</v>
       </c>
@@ -3361,7 +4566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>43892</v>
       </c>
@@ -3383,7 +4588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>43892</v>
       </c>
@@ -3405,7 +4610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>43892</v>
       </c>
@@ -3427,7 +4632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>43892</v>
       </c>
@@ -3449,7 +4654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>43892</v>
       </c>
@@ -3471,7 +4676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>43892</v>
       </c>
@@ -3493,7 +4698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>43892</v>
       </c>
@@ -3515,7 +4720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>43892</v>
       </c>
@@ -3537,7 +4742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>43901</v>
       </c>
@@ -3559,7 +4764,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>43901</v>
       </c>
@@ -3581,7 +4786,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>43902</v>
       </c>
@@ -3603,7 +4808,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>43902</v>
       </c>
@@ -3625,7 +4830,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>43902</v>
       </c>
@@ -3647,7 +4852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>43934</v>
       </c>
@@ -3669,7 +4874,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>43934</v>
       </c>
@@ -3691,7 +4896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>43934</v>
       </c>
@@ -3712,7 +4917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>43934</v>
       </c>
@@ -3733,7 +4938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
         <v>43934</v>
       </c>
@@ -3754,7 +4959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
         <v>43934</v>
       </c>
@@ -3775,7 +4980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <v>43936</v>
       </c>
@@ -3797,7 +5002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="6">
         <v>43936</v>
       </c>
@@ -3819,7 +5024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="6">
         <v>43936</v>
       </c>
@@ -3841,7 +5046,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="6">
         <v>43938</v>
       </c>
@@ -3863,7 +5068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="6">
         <v>43938</v>
       </c>
@@ -3884,7 +5089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="6">
         <v>43938</v>
       </c>
@@ -3905,7 +5110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="6">
         <v>43938</v>
       </c>
@@ -3927,7 +5132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="6">
         <v>43941</v>
       </c>
@@ -3949,7 +5154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="6">
         <v>43941</v>
       </c>
@@ -3971,7 +5176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="6">
         <v>43943</v>
       </c>
@@ -3993,7 +5198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="6">
         <v>43943</v>
       </c>
@@ -4014,7 +5219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="6">
         <v>43943</v>
       </c>
@@ -4035,7 +5240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="6">
         <v>43943</v>
       </c>
@@ -4056,7 +5261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="6">
         <v>43943</v>
       </c>
@@ -4077,7 +5282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="6">
         <v>43943</v>
       </c>
@@ -4099,7 +5304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="6">
         <v>43943</v>
       </c>
@@ -4120,7 +5325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="6">
         <v>43945</v>
       </c>
@@ -4142,7 +5347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="6">
         <v>43948</v>
       </c>
@@ -4164,7 +5369,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="6">
         <v>43950</v>
       </c>
@@ -4186,7 +5391,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="6">
         <v>43950</v>
       </c>
@@ -4208,7 +5413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="6">
         <v>43950</v>
       </c>
@@ -4230,7 +5435,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="6">
         <v>43950</v>
       </c>
@@ -4255,7 +5460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="6">
         <v>43950</v>
       </c>
@@ -4277,7 +5482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="6">
         <v>43950</v>
       </c>
@@ -4295,6 +5500,140 @@
         <v>0.75</v>
       </c>
       <c r="G61" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" s="6">
+        <v>43952</v>
+      </c>
+      <c r="B62" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" t="s">
+        <v>17</v>
+      </c>
+      <c r="D62" t="s">
+        <v>46</v>
+      </c>
+      <c r="E62">
+        <v>-0.5</v>
+      </c>
+      <c r="F62" s="5">
+        <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G62" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" s="6">
+        <v>43952</v>
+      </c>
+      <c r="B63" t="s">
+        <v>19</v>
+      </c>
+      <c r="C63" t="s">
+        <v>48</v>
+      </c>
+      <c r="E63">
+        <v>-0.75</v>
+      </c>
+      <c r="F63" s="5">
+        <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G63" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" s="6">
+        <v>43952</v>
+      </c>
+      <c r="B64" t="s">
+        <v>19</v>
+      </c>
+      <c r="C64" t="s">
+        <v>49</v>
+      </c>
+      <c r="E64">
+        <v>-0.75</v>
+      </c>
+      <c r="F64" s="5">
+        <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G64" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65" s="6">
+        <v>43952</v>
+      </c>
+      <c r="B65" t="s">
+        <v>19</v>
+      </c>
+      <c r="C65" t="s">
+        <v>50</v>
+      </c>
+      <c r="E65">
+        <v>0.5</v>
+      </c>
+      <c r="F65" s="5">
+        <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G65" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" s="6">
+        <v>43952</v>
+      </c>
+      <c r="B66" t="s">
+        <v>27</v>
+      </c>
+      <c r="C66" t="s">
+        <v>28</v>
+      </c>
+      <c r="E66">
+        <v>-0.5</v>
+      </c>
+      <c r="F66" s="5">
+        <v>-0.5</v>
+      </c>
+      <c r="G66" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" s="6">
+        <v>43952</v>
+      </c>
+      <c r="B67" t="s">
+        <v>19</v>
+      </c>
+      <c r="C67" t="s">
+        <v>51</v>
+      </c>
+      <c r="E67">
+        <v>0.5</v>
+      </c>
+      <c r="F67" s="5">
+        <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G67" s="5">
         <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
         <v>0</v>
       </c>
@@ -4310,22 +5649,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A3:M33"/>
+  <dimension ref="A3:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="4.88671875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>41</v>
       </c>
@@ -4333,7 +5673,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>42</v>
       </c>
@@ -4370,11 +5710,14 @@
       <c r="L4" s="9">
         <v>43950</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="M4" s="9">
+        <v>43952</v>
+      </c>
+      <c r="N4" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -4395,11 +5738,12 @@
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
-      <c r="M5" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M5" s="5"/>
+      <c r="N5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -4431,10 +5775,13 @@
         <v>-4</v>
       </c>
       <c r="M6" s="5">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>-0.5</v>
+      </c>
+      <c r="N6" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>12</v>
       </c>
@@ -4453,11 +5800,12 @@
       <c r="L7" s="5">
         <v>-3</v>
       </c>
-      <c r="M7" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M7" s="5"/>
+      <c r="N7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>14</v>
       </c>
@@ -4476,11 +5824,12 @@
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
-      <c r="M8" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M8" s="5"/>
+      <c r="N8" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>17</v>
       </c>
@@ -4508,10 +5857,13 @@
         <v>0</v>
       </c>
       <c r="M9" s="5">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+        <v>-0.5</v>
+      </c>
+      <c r="N9" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>46</v>
       </c>
@@ -4529,10 +5881,13 @@
         <v>0.5</v>
       </c>
       <c r="M10" s="5">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+        <v>-0.5</v>
+      </c>
+      <c r="N10" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>47</v>
       </c>
@@ -4559,11 +5914,12 @@
       <c r="L11" s="5">
         <v>-0.5</v>
       </c>
-      <c r="M11" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M11" s="5"/>
+      <c r="N11" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>11</v>
       </c>
@@ -4582,11 +5938,12 @@
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
-      <c r="M12" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M12" s="5"/>
+      <c r="N12" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>10</v>
       </c>
@@ -4605,11 +5962,12 @@
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
-      <c r="M13" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M13" s="5"/>
+      <c r="N13" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>13</v>
       </c>
@@ -4628,11 +5986,12 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
-      <c r="M14" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M14" s="5"/>
+      <c r="N14" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>16</v>
       </c>
@@ -4651,11 +6010,12 @@
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
-      <c r="M15" s="5">
+      <c r="M15" s="5"/>
+      <c r="N15" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>15</v>
       </c>
@@ -4674,11 +6034,12 @@
       <c r="L16" s="5">
         <v>-1</v>
       </c>
-      <c r="M16" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M16" s="5"/>
+      <c r="N16" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>19</v>
       </c>
@@ -4702,10 +6063,13 @@
         <v>1.5</v>
       </c>
       <c r="M17" s="5">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+        <v>-0.5</v>
+      </c>
+      <c r="N17" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>20</v>
       </c>
@@ -4724,178 +6088,180 @@
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
-      <c r="M18" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>47</v>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="B19" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="5">
-        <v>-1</v>
-      </c>
-      <c r="G19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5">
+        <v>-3</v>
+      </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
-      <c r="M19" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M19" s="5"/>
+      <c r="N19" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B20" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
-      <c r="M20" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
-        <v>47</v>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="B21" s="5">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
+      <c r="F21" s="5">
+        <v>0.5</v>
+      </c>
       <c r="G21" s="5">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
-      <c r="M21" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M21" s="5"/>
+      <c r="N21" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="5">
-        <v>1</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="5">
-        <v>-1</v>
-      </c>
+      <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
+      <c r="L22" s="5">
+        <v>0.75</v>
+      </c>
       <c r="M22" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B23" s="5">
-        <v>1</v>
-      </c>
+        <v>-0.75</v>
+      </c>
+      <c r="N22" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="5">
-        <v>-1</v>
-      </c>
+      <c r="G23" s="5"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
+      <c r="L23" s="5">
+        <v>0.75</v>
+      </c>
       <c r="M23" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="5">
-        <v>0.5</v>
-      </c>
+        <v>-0.75</v>
+      </c>
+      <c r="N23" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
-      <c r="F24" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="G24" s="5">
-        <v>-1</v>
-      </c>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="5">
         <v>0.5</v>
       </c>
+      <c r="N24" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
-      <c r="F25" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="G25" s="5">
-        <v>-1</v>
-      </c>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
-        <v>48</v>
+        <v>0.5</v>
+      </c>
+      <c r="N25" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" s="12" t="s">
+        <v>47</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -4907,60 +6273,73 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
-      <c r="L26" s="5">
-        <v>0.75</v>
-      </c>
+      <c r="L26" s="5"/>
       <c r="M26" s="5">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" s="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="N26" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="5">
+        <v>2.5</v>
+      </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
+      <c r="E27" s="5">
+        <v>-1</v>
+      </c>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
+      <c r="I27" s="5">
+        <v>-1.5</v>
+      </c>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
-      <c r="L27" s="5">
-        <v>0.75</v>
-      </c>
-      <c r="M27" s="5">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5">
+        <v>5.5</v>
+      </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
+      <c r="E28" s="5">
+        <v>-4.5</v>
+      </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
-      <c r="L28" s="5">
-        <v>0.75</v>
-      </c>
+      <c r="L28" s="5"/>
       <c r="M28" s="5">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B29" s="5"/>
+        <v>-0.5</v>
+      </c>
+      <c r="N28" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5">
+        <v>1</v>
+      </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
@@ -4970,49 +6349,49 @@
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
-      <c r="L29" s="5">
-        <v>0.75</v>
-      </c>
+      <c r="L29" s="5"/>
       <c r="M29" s="5">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>23</v>
+        <v>-0.5</v>
+      </c>
+      <c r="N29" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="B30" s="5">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
-      <c r="I30" s="5">
-        <v>-1.5</v>
-      </c>
+      <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
-      <c r="M30" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>27</v>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="B31" s="5">
-        <v>5.5</v>
+        <v>1.5</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5">
-        <v>-4.5</v>
+        <v>-1.5</v>
       </c>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
@@ -5021,11 +6400,12 @@
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
-      <c r="M31" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M31" s="5"/>
+      <c r="N31" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>31</v>
       </c>
@@ -5046,11 +6426,12 @@
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
-      <c r="M32" s="5">
+      <c r="M32" s="5"/>
+      <c r="N32" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>43</v>
       </c>
@@ -5088,7 +6469,10 @@
         <v>-2.5</v>
       </c>
       <c r="M33" s="5">
-        <v>6</v>
+        <v>-1.5</v>
+      </c>
+      <c r="N33" s="5">
+        <v>4.5</v>
       </c>
     </row>
   </sheetData>
@@ -5098,23 +6482,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A3:H15"/>
+  <dimension ref="A3:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -5134,7 +6518,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>43892</v>
       </c>
@@ -5157,7 +6541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>43901</v>
       </c>
@@ -5180,7 +6564,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>43902</v>
       </c>
@@ -5203,7 +6587,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>43934</v>
       </c>
@@ -5226,7 +6610,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>43936</v>
       </c>
@@ -5249,7 +6633,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>43938</v>
       </c>
@@ -5272,7 +6656,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>43941</v>
       </c>
@@ -5295,7 +6679,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>43943</v>
       </c>
@@ -5318,7 +6702,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>43945</v>
       </c>
@@ -5341,7 +6725,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>43948</v>
       </c>
@@ -5364,7 +6748,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>43950</v>
       </c>
@@ -5387,12 +6771,35 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F15" s="7">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>43952</v>
+      </c>
+      <c r="B15" s="5">
+        <v>28</v>
+      </c>
+      <c r="C15" s="5">
+        <v>23.5</v>
+      </c>
+      <c r="F15" s="6">
+        <f t="shared" ref="F15" si="25">A15</f>
+        <v>43952</v>
+      </c>
+      <c r="G15">
+        <f t="shared" ref="G15" si="26">B15</f>
+        <v>28</v>
+      </c>
+      <c r="H15">
+        <f t="shared" ref="H15" si="27">C15</f>
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F16" s="7">
         <v>44013</v>
       </c>
-      <c r="G15">
-        <v>27.5</v>
+      <c r="G16">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated burnup and README for meeting!
</commit_message>
<xml_diff>
--- a/misc/klask-burn-up.xlsx
+++ b/misc/klask-burn-up.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valer\Documents\GitHub\klask\misc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trevo\OneDrive\Documents\GitHub\klask\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F48908-E863-428D-A6C3-11FA3AB5C6C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD6EE63-8E62-4117-9D00-83ECEB0D00D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data-entry" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="24" r:id="rId4"/>
+    <pivotCache cacheId="6" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -181,9 +181,6 @@
     <t>fix-hard-coding</t>
   </si>
   <si>
-    <t>(blank)</t>
-  </si>
-  <si>
     <t>most-loc-points</t>
   </si>
   <si>
@@ -218,24 +215,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -250,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -263,19 +248,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1648,7 +1621,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1686,10 +1659,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'burn-up'!$F$4:$F$16</c:f>
+              <c:f>'burn-up'!$F$4:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>43892</c:v>
                 </c:pt>
@@ -1726,7 +1699,10 @@
                 <c:pt idx="11">
                   <c:v>43952</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="d\-mmm">
+                <c:pt idx="12">
+                  <c:v>43959</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="d\-mmm">
                   <c:v>44013</c:v>
                 </c:pt>
               </c:numCache>
@@ -1734,10 +1710,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'burn-up'!$G$4:$G$16</c:f>
+              <c:f>'burn-up'!$G$4:$G$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>39.5</c:v>
                 </c:pt>
@@ -1775,6 +1751,9 @@
                   <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
@@ -1830,10 +1809,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>'burn-up'!$F$4:$F$16</c:f>
+              <c:f>'burn-up'!$F$4:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>43892</c:v>
                 </c:pt>
@@ -1870,7 +1849,10 @@
                 <c:pt idx="11">
                   <c:v>43952</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="d\-mmm">
+                <c:pt idx="12">
+                  <c:v>43959</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="d\-mmm">
                   <c:v>44013</c:v>
                 </c:pt>
               </c:numCache>
@@ -1878,10 +1860,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'burn-up'!$H$4:$H$15</c:f>
+              <c:f>'burn-up'!$H$4:$H$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1917,6 +1899,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>23.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1996,7 +1981,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="472556976"/>
@@ -2056,7 +2041,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="472557808"/>
@@ -2097,7 +2082,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2668,16 +2653,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>518160</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>74295</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>241935</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>150495</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2706,13 +2691,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Valeria Welsh" refreshedDate="43952.631736342591" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="66" xr:uid="{00000000-000A-0000-FFFF-FFFF39000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Trevor Moldenhauer" refreshedDate="43959.619217361113" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="70" xr:uid="{00000000-000A-0000-FFFF-FFFF39000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
   <cacheFields count="7">
     <cacheField name="Date" numFmtId="14">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2020-03-02T00:00:00" maxDate="2020-05-02T00:00:00" count="14">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2020-03-02T00:00:00" maxDate="2020-05-09T00:00:00" count="15">
         <d v="2020-03-02T00:00:00"/>
         <d v="2020-03-11T00:00:00"/>
         <d v="2020-03-12T00:00:00"/>
@@ -2725,6 +2710,7 @@
         <d v="2020-04-27T00:00:00"/>
         <d v="2020-04-29T00:00:00"/>
         <d v="2020-05-01T00:00:00"/>
+        <d v="2020-05-08T00:00:00"/>
         <d v="2020-03-26T00:00:00" u="1"/>
         <d v="2020-03-30T00:00:00" u="1"/>
       </sharedItems>
@@ -2799,7 +2785,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="66">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="70">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -3394,20 +3380,56 @@
     <n v="0.5"/>
     <n v="0"/>
   </r>
+  <r>
+    <x v="12"/>
+    <x v="1"/>
+    <x v="10"/>
+    <x v="0"/>
+    <n v="-1"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="2"/>
+    <x v="29"/>
+    <x v="0"/>
+    <n v="-0.5"/>
+    <n v="0"/>
+    <n v="0.5"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="2"/>
+    <x v="28"/>
+    <x v="0"/>
+    <n v="-0.5"/>
+    <n v="0"/>
+    <n v="0.5"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="5"/>
+    <x v="23"/>
+    <x v="0"/>
+    <n v="-1"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="total" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="work-buckets" colHeaderCaption="date">
-  <location ref="A3:N33" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="total" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="work-buckets" colHeaderCaption="date">
+  <location ref="A3:O11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisCol" numFmtId="164" showAll="0">
-      <items count="15">
+      <items count="16">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
-        <item m="1" x="12"/>
         <item m="1" x="13"/>
+        <item m="1" x="14"/>
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
@@ -3417,16 +3439,17 @@
         <item x="9"/>
         <item x="10"/>
         <item x="11"/>
+        <item x="12"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisRow" showAll="0">
       <items count="7">
         <item sd="0" x="0"/>
-        <item x="1"/>
-        <item x="2"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
         <item sd="0" x="3"/>
-        <item x="4"/>
+        <item sd="0" x="4"/>
         <item sd="0" x="5"/>
         <item t="default"/>
       </items>
@@ -3463,7 +3486,7 @@
         <item sd="0" x="26"/>
         <item sd="0" x="27"/>
         <item sd="0" x="28"/>
-        <item x="29"/>
+        <item sd="0" x="29"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -3483,87 +3506,21 @@
     <field x="2"/>
     <field x="3"/>
   </rowFields>
-  <rowItems count="29">
+  <rowItems count="7">
     <i>
       <x/>
     </i>
     <i>
       <x v="1"/>
     </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i r="1">
-      <x v="8"/>
-    </i>
-    <i r="1">
-      <x v="10"/>
-    </i>
-    <i r="1">
-      <x v="11"/>
-    </i>
     <i>
       <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="12"/>
-    </i>
-    <i r="1">
-      <x v="13"/>
-    </i>
-    <i r="1">
-      <x v="14"/>
-    </i>
-    <i r="1">
-      <x v="26"/>
-    </i>
-    <i r="1">
-      <x v="27"/>
-    </i>
-    <i r="1">
-      <x v="28"/>
-    </i>
-    <i r="1">
-      <x v="29"/>
-    </i>
-    <i r="1">
-      <x v="30"/>
-    </i>
-    <i r="2">
-      <x v="1"/>
     </i>
     <i>
       <x v="3"/>
     </i>
     <i>
       <x v="4"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i r="1">
-      <x v="20"/>
-    </i>
-    <i r="1">
-      <x v="21"/>
     </i>
     <i>
       <x v="5"/>
@@ -3575,7 +3532,7 @@
   <colFields count="1">
     <field x="0"/>
   </colFields>
-  <colItems count="13">
+  <colItems count="14">
     <i>
       <x/>
     </i>
@@ -3611,6 +3568,9 @@
     </i>
     <i>
       <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
     </i>
     <i t="grand">
       <x/>
@@ -3773,16 +3733,16 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable3" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:C15" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable3" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C16" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" numFmtId="14" showAll="0">
-      <items count="15">
+      <items count="16">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
-        <item m="1" x="12"/>
         <item m="1" x="13"/>
+        <item m="1" x="14"/>
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
@@ -3792,6 +3752,7 @@
         <item x="9"/>
         <item x="10"/>
         <item x="11"/>
+        <item x="12"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -3805,7 +3766,7 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="12">
+  <rowItems count="13">
     <i>
       <x/>
     </i>
@@ -3842,6 +3803,9 @@
     <i>
       <x v="13"/>
     </i>
+    <i>
+      <x v="14"/>
+    </i>
   </rowItems>
   <colFields count="1">
     <field x="-2"/>
@@ -3871,8 +3835,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G67" totalsRowShown="0">
-  <autoFilter ref="A1:G67" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G71" totalsRowShown="0">
+  <autoFilter ref="A1:G71" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="194"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="level-1"/>
@@ -4153,23 +4117,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="F67" sqref="F67"/>
+      <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4192,7 +4156,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43892</v>
       </c>
@@ -4214,7 +4178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43892</v>
       </c>
@@ -4236,7 +4200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43892</v>
       </c>
@@ -4258,7 +4222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43892</v>
       </c>
@@ -4280,7 +4244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43892</v>
       </c>
@@ -4302,7 +4266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43892</v>
       </c>
@@ -4324,7 +4288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43892</v>
       </c>
@@ -4346,7 +4310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43892</v>
       </c>
@@ -4368,7 +4332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43892</v>
       </c>
@@ -4390,7 +4354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43892</v>
       </c>
@@ -4412,7 +4376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43892</v>
       </c>
@@ -4434,7 +4398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43892</v>
       </c>
@@ -4456,7 +4420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43892</v>
       </c>
@@ -4478,7 +4442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43892</v>
       </c>
@@ -4500,7 +4464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43892</v>
       </c>
@@ -4522,7 +4486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43892</v>
       </c>
@@ -4544,7 +4508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43892</v>
       </c>
@@ -4566,7 +4530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43892</v>
       </c>
@@ -4588,7 +4552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43892</v>
       </c>
@@ -4610,7 +4574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43892</v>
       </c>
@@ -4632,7 +4596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43892</v>
       </c>
@@ -4654,7 +4618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43892</v>
       </c>
@@ -4676,7 +4640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43892</v>
       </c>
@@ -4698,7 +4662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43892</v>
       </c>
@@ -4720,7 +4684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43892</v>
       </c>
@@ -4742,7 +4706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43901</v>
       </c>
@@ -4764,7 +4728,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43901</v>
       </c>
@@ -4786,7 +4750,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43902</v>
       </c>
@@ -4808,7 +4772,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43902</v>
       </c>
@@ -4830,7 +4794,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>43902</v>
       </c>
@@ -4852,7 +4816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>43934</v>
       </c>
@@ -4874,7 +4838,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>43934</v>
       </c>
@@ -4896,7 +4860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>43934</v>
       </c>
@@ -4917,7 +4881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>43934</v>
       </c>
@@ -4938,7 +4902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>43934</v>
       </c>
@@ -4959,7 +4923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>43934</v>
       </c>
@@ -4980,7 +4944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>43936</v>
       </c>
@@ -5002,7 +4966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>43936</v>
       </c>
@@ -5024,7 +4988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>43936</v>
       </c>
@@ -5046,7 +5010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>43938</v>
       </c>
@@ -5068,7 +5032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>43938</v>
       </c>
@@ -5089,7 +5053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>43938</v>
       </c>
@@ -5110,7 +5074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>43938</v>
       </c>
@@ -5132,7 +5096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>43941</v>
       </c>
@@ -5154,7 +5118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>43941</v>
       </c>
@@ -5176,7 +5140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>43943</v>
       </c>
@@ -5198,7 +5162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>43943</v>
       </c>
@@ -5219,7 +5183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>43943</v>
       </c>
@@ -5240,7 +5204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <v>43943</v>
       </c>
@@ -5261,7 +5225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
         <v>43943</v>
       </c>
@@ -5282,7 +5246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="6">
         <v>43943</v>
       </c>
@@ -5304,7 +5268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="6">
         <v>43943</v>
       </c>
@@ -5325,7 +5289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
         <v>43945</v>
       </c>
@@ -5347,7 +5311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
         <v>43948</v>
       </c>
@@ -5369,7 +5333,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
         <v>43950</v>
       </c>
@@ -5391,7 +5355,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="6">
         <v>43950</v>
       </c>
@@ -5413,7 +5377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="6">
         <v>43950</v>
       </c>
@@ -5435,7 +5399,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="6">
         <v>43950</v>
       </c>
@@ -5460,7 +5424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="6">
         <v>43950</v>
       </c>
@@ -5468,7 +5432,7 @@
         <v>19</v>
       </c>
       <c r="C60" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E60">
         <v>0.75</v>
@@ -5482,7 +5446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="6">
         <v>43950</v>
       </c>
@@ -5490,7 +5454,7 @@
         <v>19</v>
       </c>
       <c r="C61" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E61">
         <v>0.75</v>
@@ -5504,7 +5468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="6">
         <v>43952</v>
       </c>
@@ -5529,7 +5493,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="6">
         <v>43952</v>
       </c>
@@ -5537,7 +5501,7 @@
         <v>19</v>
       </c>
       <c r="C63" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E63">
         <v>-0.75</v>
@@ -5551,7 +5515,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="6">
         <v>43952</v>
       </c>
@@ -5559,7 +5523,7 @@
         <v>19</v>
       </c>
       <c r="C64" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E64">
         <v>-0.75</v>
@@ -5573,7 +5537,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="6">
         <v>43952</v>
       </c>
@@ -5581,7 +5545,7 @@
         <v>19</v>
       </c>
       <c r="C65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E65">
         <v>0.5</v>
@@ -5595,7 +5559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="6">
         <v>43952</v>
       </c>
@@ -5616,7 +5580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="6">
         <v>43952</v>
       </c>
@@ -5624,7 +5588,7 @@
         <v>19</v>
       </c>
       <c r="C67" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E67">
         <v>0.5</v>
@@ -5636,6 +5600,94 @@
       <c r="G67" s="5">
         <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="6">
+        <v>43959</v>
+      </c>
+      <c r="B68" t="s">
+        <v>9</v>
+      </c>
+      <c r="C68" t="s">
+        <v>16</v>
+      </c>
+      <c r="E68">
+        <v>-1</v>
+      </c>
+      <c r="F68" s="5">
+        <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G68" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="6">
+        <v>43959</v>
+      </c>
+      <c r="B69" t="s">
+        <v>19</v>
+      </c>
+      <c r="C69" t="s">
+        <v>50</v>
+      </c>
+      <c r="E69">
+        <v>-0.5</v>
+      </c>
+      <c r="F69" s="5">
+        <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G69" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="6">
+        <v>43959</v>
+      </c>
+      <c r="B70" t="s">
+        <v>19</v>
+      </c>
+      <c r="C70" t="s">
+        <v>49</v>
+      </c>
+      <c r="E70">
+        <v>-0.5</v>
+      </c>
+      <c r="F70" s="5">
+        <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G70" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="6">
+        <v>43959</v>
+      </c>
+      <c r="B71" t="s">
+        <v>31</v>
+      </c>
+      <c r="C71" t="s">
+        <v>33</v>
+      </c>
+      <c r="E71">
+        <v>-1</v>
+      </c>
+      <c r="F71" s="5">
+        <f>IF(Table1[[#This Row],[size-delta]]&gt;0,Table1[[#This Row],[size-delta]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G71" s="5">
+        <f>Table1[[#This Row],[release-target]]-Table1[[#This Row],[size-delta]]</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5649,23 +5701,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A3:N33"/>
+  <dimension ref="A3:O11"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>41</v>
       </c>
@@ -5673,51 +5725,54 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>43892</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>43901</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>43902</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>43934</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="8">
         <v>43936</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="8">
         <v>43938</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="8">
         <v>43941</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="8">
         <v>43943</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="8">
         <v>43945</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="8">
         <v>43948</v>
       </c>
-      <c r="L4" s="9">
+      <c r="L4" s="8">
         <v>43950</v>
       </c>
-      <c r="M4" s="9">
+      <c r="M4" s="8">
         <v>43952</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="N4" s="8">
+        <v>43959</v>
+      </c>
+      <c r="O4" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -5739,11 +5794,12 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N5" s="5"/>
+      <c r="O5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -5778,132 +5834,155 @@
         <v>-0.5</v>
       </c>
       <c r="N6" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
-        <v>12</v>
+        <v>-1</v>
+      </c>
+      <c r="O6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="B7" s="5">
-        <v>3</v>
+        <v>5.5</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="F7" s="5">
+        <v>-0.5</v>
+      </c>
+      <c r="G7" s="5">
+        <v>-5</v>
+      </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5">
-        <v>-3</v>
-      </c>
-      <c r="M7" s="5"/>
+        <v>1.5</v>
+      </c>
+      <c r="M7" s="5">
+        <v>-0.5</v>
+      </c>
       <c r="N7" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
-        <v>14</v>
+        <v>-1</v>
+      </c>
+      <c r="O7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="B8" s="5">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="E8" s="5">
+        <v>-1</v>
+      </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5">
-        <v>-2</v>
+        <v>-1.5</v>
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
-      <c r="N8" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
-        <v>17</v>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="B9" s="5">
-        <v>3</v>
+        <v>5.5</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="E9" s="5">
+        <v>-4.5</v>
+      </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="5">
-        <v>0</v>
-      </c>
-      <c r="I9" s="5">
-        <v>-1</v>
-      </c>
-      <c r="J9" s="5">
-        <v>0</v>
-      </c>
-      <c r="K9" s="5">
-        <v>-1.5</v>
-      </c>
-      <c r="L9" s="5">
-        <v>0</v>
-      </c>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
       <c r="M9" s="5">
         <v>-0.5</v>
       </c>
-      <c r="N9" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="5">
+        <v>6.5</v>
+      </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="E10" s="5">
+        <v>-1.5</v>
+      </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
+      <c r="I10" s="5">
+        <v>-3</v>
+      </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
-      <c r="L10" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="M10" s="5">
-        <v>-0.5</v>
-      </c>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
       <c r="N10" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
-        <v>47</v>
+        <v>-1</v>
+      </c>
+      <c r="O10" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="B11" s="5">
-        <v>3</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+        <v>39.5</v>
+      </c>
+      <c r="C11" s="5">
+        <v>-3.5</v>
+      </c>
+      <c r="D11" s="5">
+        <v>-2</v>
+      </c>
+      <c r="E11" s="5">
+        <v>-7</v>
+      </c>
+      <c r="F11" s="5">
+        <v>-2.5</v>
+      </c>
+      <c r="G11" s="5">
+        <v>-6</v>
+      </c>
       <c r="H11" s="5">
         <v>0</v>
       </c>
       <c r="I11" s="5">
-        <v>-1</v>
+        <v>-8.5</v>
       </c>
       <c r="J11" s="5">
         <v>0</v>
@@ -5912,567 +5991,16 @@
         <v>-1.5</v>
       </c>
       <c r="L11" s="5">
-        <v>-0.5</v>
-      </c>
-      <c r="M11" s="5"/>
+        <v>-2.5</v>
+      </c>
+      <c r="M11" s="5">
+        <v>-1.5</v>
+      </c>
       <c r="N11" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="5">
-        <v>1</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5">
-        <v>-1</v>
-      </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="5">
-        <v>1</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5">
-        <v>-1</v>
-      </c>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5">
-        <v>2</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5">
-        <v>-2</v>
-      </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="5">
-        <v>1</v>
-      </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5">
-        <v>0</v>
-      </c>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="5">
-        <v>1</v>
-      </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5">
-        <v>-1</v>
-      </c>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="5">
-        <v>5.5</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5">
-        <v>-0.5</v>
-      </c>
-      <c r="G17" s="5">
-        <v>-5</v>
-      </c>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5">
+        <v>-3</v>
+      </c>
+      <c r="O11" s="5">
         <v>1.5</v>
-      </c>
-      <c r="M17" s="5">
-        <v>-0.5</v>
-      </c>
-      <c r="N17" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="5">
-        <v>1</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5">
-        <v>-1</v>
-      </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="5">
-        <v>3</v>
-      </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5">
-        <v>-3</v>
-      </c>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="5">
-        <v>1</v>
-      </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5">
-        <v>-1</v>
-      </c>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="G21" s="5">
-        <v>-1</v>
-      </c>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5">
-        <v>0.75</v>
-      </c>
-      <c r="M22" s="5">
-        <v>-0.75</v>
-      </c>
-      <c r="N22" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5">
-        <v>0.75</v>
-      </c>
-      <c r="M23" s="5">
-        <v>-0.75</v>
-      </c>
-      <c r="N23" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="N24" s="5">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="N25" s="5">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="N26" s="5">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5">
-        <v>-1</v>
-      </c>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5">
-        <v>-1.5</v>
-      </c>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B28" s="5">
-        <v>5.5</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5">
-        <v>-4.5</v>
-      </c>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="5">
-        <v>-0.5</v>
-      </c>
-      <c r="N28" s="5">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A29" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="5">
-        <v>1</v>
-      </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5">
-        <v>-0.5</v>
-      </c>
-      <c r="N29" s="5">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="5">
-        <v>3</v>
-      </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5">
-        <v>-3</v>
-      </c>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A31" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5">
-        <v>-1.5</v>
-      </c>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32" s="5">
-        <v>6.5</v>
-      </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5">
-        <v>-1.5</v>
-      </c>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5">
-        <v>-3</v>
-      </c>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B33" s="5">
-        <v>39.5</v>
-      </c>
-      <c r="C33" s="5">
-        <v>-3.5</v>
-      </c>
-      <c r="D33" s="5">
-        <v>-2</v>
-      </c>
-      <c r="E33" s="5">
-        <v>-7</v>
-      </c>
-      <c r="F33" s="5">
-        <v>-2.5</v>
-      </c>
-      <c r="G33" s="5">
-        <v>-6</v>
-      </c>
-      <c r="H33" s="5">
-        <v>0</v>
-      </c>
-      <c r="I33" s="5">
-        <v>-8.5</v>
-      </c>
-      <c r="J33" s="5">
-        <v>0</v>
-      </c>
-      <c r="K33" s="5">
-        <v>-1.5</v>
-      </c>
-      <c r="L33" s="5">
-        <v>-2.5</v>
-      </c>
-      <c r="M33" s="5">
-        <v>-1.5</v>
-      </c>
-      <c r="N33" s="5">
-        <v>4.5</v>
       </c>
     </row>
   </sheetData>
@@ -6482,23 +6010,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A3:H16"/>
+  <dimension ref="A3:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -6518,7 +6046,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>43892</v>
       </c>
@@ -6541,7 +6069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>43901</v>
       </c>
@@ -6564,7 +6092,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>43902</v>
       </c>
@@ -6587,7 +6115,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>43934</v>
       </c>
@@ -6610,7 +6138,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>43936</v>
       </c>
@@ -6633,7 +6161,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>43938</v>
       </c>
@@ -6656,7 +6184,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>43941</v>
       </c>
@@ -6679,7 +6207,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>43943</v>
       </c>
@@ -6702,7 +6230,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>43945</v>
       </c>
@@ -6725,7 +6253,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>43948</v>
       </c>
@@ -6748,7 +6276,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>43950</v>
       </c>
@@ -6771,7 +6299,7 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>43952</v>
       </c>
@@ -6794,11 +6322,34 @@
         <v>23.5</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F16" s="7">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>43959</v>
+      </c>
+      <c r="B16" s="5">
+        <v>28</v>
+      </c>
+      <c r="C16" s="5">
+        <v>26.5</v>
+      </c>
+      <c r="F16" s="6">
+        <f t="shared" ref="F16" si="28">A16</f>
+        <v>43959</v>
+      </c>
+      <c r="G16">
+        <f t="shared" ref="G16" si="29">B16</f>
+        <v>28</v>
+      </c>
+      <c r="H16">
+        <f t="shared" ref="H16" si="30">C16</f>
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F17" s="7">
         <v>44013</v>
       </c>
-      <c r="G16">
+      <c r="G17">
         <v>28</v>
       </c>
     </row>

</xml_diff>